<commit_message>
Update Excel file and remove temporary file
</commit_message>
<xml_diff>
--- a/public/expense-analysis.xlsx
+++ b/public/expense-analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/Library/Mobile Documents/com~apple~CloudDocs/Gilliam/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-gilliam-roanoke-1/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1DC99B0-09AA-CC40-9B0B-75DF59A55B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7D48C3-2420-6544-8C2F-E55C1748CC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="20120" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="107">
   <si>
     <t>Category</t>
   </si>
@@ -304,12 +304,6 @@
     <t>Medical Supplies</t>
   </si>
   <si>
-    <t>Gross Profit</t>
-  </si>
-  <si>
-    <t>Net Ordinary Income</t>
-  </si>
-  <si>
     <t>Clamped</t>
   </si>
   <si>
@@ -322,6 +316,12 @@
     <t>One-time</t>
   </si>
   <si>
+    <t>Costs Declined Despite Profit Growth</t>
+  </si>
+  <si>
+    <t>Costs Grew Slower than Profit</t>
+  </si>
+  <si>
     <t>Below Threshold</t>
   </si>
   <si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Under-Leveraged</t>
+  </si>
+  <si>
+    <t>Expense Growth Alignment</t>
   </si>
 </sst>
 </file>
@@ -705,13 +708,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC68"/>
+  <dimension ref="A1:AD66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -779,28 +812,31 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -841,13 +877,13 @@
         <v>1053.8418543645289</v>
       </c>
       <c r="N2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O2">
         <v>626.65200000000004</v>
       </c>
       <c r="P2">
-        <v>284.68113192125611</v>
+        <v>379.59741842599612</v>
       </c>
       <c r="Q2">
         <v>626.65200000000004</v>
@@ -867,8 +903,8 @@
       <c r="V2">
         <v>-125.7704011981041</v>
       </c>
-      <c r="X2" t="s">
-        <v>100</v>
+      <c r="W2" t="s">
+        <v>98</v>
       </c>
       <c r="Y2" t="s">
         <v>100</v>
@@ -877,13 +913,16 @@
         <v>100</v>
       </c>
       <c r="AA2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB2" t="s">
         <v>103</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -924,13 +963,13 @@
         <v>1053.8418543645289</v>
       </c>
       <c r="N3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O3">
         <v>626.65200000000004</v>
       </c>
       <c r="P3">
-        <v>284.68113192125611</v>
+        <v>379.59741842599612</v>
       </c>
       <c r="Q3">
         <v>626.65200000000004</v>
@@ -950,8 +989,8 @@
       <c r="V3">
         <v>-125.7704011981041</v>
       </c>
-      <c r="X3" t="s">
-        <v>100</v>
+      <c r="W3" t="s">
+        <v>98</v>
       </c>
       <c r="Y3" t="s">
         <v>100</v>
@@ -960,13 +999,16 @@
         <v>100</v>
       </c>
       <c r="AA3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB3" t="s">
         <v>103</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1007,13 +1049,13 @@
         <v>1215.905209574297</v>
       </c>
       <c r="N4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O4">
         <v>-5344.93</v>
       </c>
       <c r="P4">
-        <v>-2428.143088093359</v>
+        <v>-3237.7166747535471</v>
       </c>
       <c r="Q4">
         <v>-5344.93</v>
@@ -1033,8 +1075,8 @@
       <c r="V4">
         <v>6.0203868911808678E-2</v>
       </c>
-      <c r="X4" t="s">
-        <v>100</v>
+      <c r="W4" t="s">
+        <v>99</v>
       </c>
       <c r="Y4" t="s">
         <v>100</v>
@@ -1045,11 +1087,14 @@
       <c r="AA4" t="s">
         <v>100</v>
       </c>
-      <c r="AC4">
+      <c r="AB4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1090,13 +1135,13 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O5">
         <v>493.75200000000012</v>
       </c>
       <c r="P5">
-        <v>224.3061192629786</v>
+        <v>299.09261367181858</v>
       </c>
       <c r="Q5">
         <v>493.75200000000012</v>
@@ -1116,8 +1161,8 @@
       <c r="V5">
         <v>-0.45404564609826009</v>
       </c>
-      <c r="X5" t="s">
-        <v>100</v>
+      <c r="W5" t="s">
+        <v>98</v>
       </c>
       <c r="Y5" t="s">
         <v>100</v>
@@ -1128,11 +1173,14 @@
       <c r="AA5" t="s">
         <v>100</v>
       </c>
-      <c r="AC5">
+      <c r="AB5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1173,13 +1221,13 @@
         <v>-12.743006246802681</v>
       </c>
       <c r="N6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O6">
         <v>281.98399999999998</v>
       </c>
       <c r="P6">
-        <v>128.10223904764291</v>
+        <v>170.81314419715591</v>
       </c>
       <c r="Q6">
         <v>281.98399999999998</v>
@@ -1199,8 +1247,8 @@
       <c r="V6">
         <v>-0.58190788706878993</v>
       </c>
-      <c r="X6" t="s">
-        <v>100</v>
+      <c r="W6" t="s">
+        <v>98</v>
       </c>
       <c r="Y6" t="s">
         <v>100</v>
@@ -1211,11 +1259,14 @@
       <c r="AA6" t="s">
         <v>100</v>
       </c>
-      <c r="AC6">
+      <c r="AB6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1256,13 +1307,13 @@
         <v>60.235031218222097</v>
       </c>
       <c r="N7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O7">
         <v>104.79600000000001</v>
       </c>
       <c r="P7">
-        <v>47.607673638351038</v>
+        <v>63.480673581781737</v>
       </c>
       <c r="Q7">
         <v>104.79600000000001</v>
@@ -1282,8 +1333,8 @@
       <c r="V7">
         <v>-1.210177060389181</v>
       </c>
-      <c r="X7" t="s">
-        <v>100</v>
+      <c r="W7" t="s">
+        <v>98</v>
       </c>
       <c r="Y7" t="s">
         <v>100</v>
@@ -1294,11 +1345,14 @@
       <c r="AA7" t="s">
         <v>100</v>
       </c>
-      <c r="AC7">
+      <c r="AB7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1339,13 +1393,13 @@
         <v>57.344810514279857</v>
       </c>
       <c r="N8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O8">
         <v>344.42599999999999</v>
       </c>
       <c r="P8">
-        <v>156.46895492731301</v>
+        <v>208.63768158210959</v>
       </c>
       <c r="Q8">
         <v>344.42599999999999</v>
@@ -1365,8 +1419,8 @@
       <c r="V8">
         <v>-0.231961024274254</v>
       </c>
-      <c r="X8" t="s">
-        <v>100</v>
+      <c r="W8" t="s">
+        <v>98</v>
       </c>
       <c r="Y8" t="s">
         <v>100</v>
@@ -1377,11 +1431,14 @@
       <c r="AA8" t="s">
         <v>100</v>
       </c>
-      <c r="AC8">
+      <c r="AB8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1422,13 +1479,13 @@
         <v>84.31720770385266</v>
       </c>
       <c r="N9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O9">
         <v>381.00599999999997</v>
       </c>
       <c r="P9">
-        <v>173.08684780195401</v>
+        <v>230.79618991851149</v>
       </c>
       <c r="Q9">
         <v>381.00599999999997</v>
@@ -1448,8 +1505,8 @@
       <c r="V9">
         <v>-7.0067423191985963E-5</v>
       </c>
-      <c r="X9" t="s">
-        <v>100</v>
+      <c r="W9" t="s">
+        <v>98</v>
       </c>
       <c r="Y9" t="s">
         <v>100</v>
@@ -1460,11 +1517,14 @@
       <c r="AA9" t="s">
         <v>100</v>
       </c>
-      <c r="AC9">
+      <c r="AB9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1505,13 +1565,13 @@
         <v>-0.204142920372373</v>
       </c>
       <c r="N10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O10">
         <v>5.9100445581432153</v>
       </c>
       <c r="P10">
-        <v>2.684868434980292</v>
+        <v>3.580037496176141</v>
       </c>
       <c r="Q10">
         <v>5.9100445581432153</v>
@@ -1531,8 +1591,8 @@
       <c r="V10">
         <v>0.1318279641011087</v>
       </c>
-      <c r="X10" t="s">
-        <v>100</v>
+      <c r="W10" t="s">
+        <v>99</v>
       </c>
       <c r="Y10" t="s">
         <v>100</v>
@@ -1543,11 +1603,14 @@
       <c r="AA10" t="s">
         <v>100</v>
       </c>
-      <c r="AC10">
+      <c r="AB10" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1588,13 +1651,13 @@
         <v>-24.563487227989999</v>
       </c>
       <c r="N11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O11">
         <v>100.70399999999999</v>
       </c>
       <c r="P11">
-        <v>45.748722910001362</v>
+        <v>61.00192519160796</v>
       </c>
       <c r="Q11">
         <v>100.70399999999999</v>
@@ -1614,8 +1677,8 @@
       <c r="V11">
         <v>7.9820362483175575E-2</v>
       </c>
-      <c r="X11" t="s">
-        <v>100</v>
+      <c r="W11" t="s">
+        <v>99</v>
       </c>
       <c r="Y11" t="s">
         <v>100</v>
@@ -1626,11 +1689,14 @@
       <c r="AA11" t="s">
         <v>100</v>
       </c>
-      <c r="AC11">
+      <c r="AB11" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1671,13 +1737,13 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O12">
         <v>32.770000000000003</v>
       </c>
       <c r="P12">
-        <v>14.887051653963541</v>
+        <v>19.850582782501121</v>
       </c>
       <c r="Q12">
         <v>32.770000000000003</v>
@@ -1697,8 +1763,8 @@
       <c r="V12">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X12" t="s">
-        <v>100</v>
+      <c r="W12" t="s">
+        <v>99</v>
       </c>
       <c r="Y12" t="s">
         <v>100</v>
@@ -1709,11 +1775,14 @@
       <c r="AA12" t="s">
         <v>100</v>
       </c>
-      <c r="AC12">
+      <c r="AB12" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1754,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -1780,8 +1849,8 @@
       <c r="V13">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X13" t="s">
-        <v>100</v>
+      <c r="W13" t="s">
+        <v>99</v>
       </c>
       <c r="Y13" t="s">
         <v>100</v>
@@ -1792,11 +1861,14 @@
       <c r="AA13" t="s">
         <v>100</v>
       </c>
-      <c r="AC13">
+      <c r="AB13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1837,13 +1909,13 @@
         <v>5.7030506926241458</v>
       </c>
       <c r="N14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O14">
         <v>-7.8874317955383484</v>
       </c>
       <c r="P14">
-        <v>-3.5831737734908078</v>
+        <v>-4.7778491851896678</v>
       </c>
       <c r="Q14">
         <v>-7.8874317955383484</v>
@@ -1863,8 +1935,8 @@
       <c r="V14">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X14" t="s">
-        <v>100</v>
+      <c r="W14" t="s">
+        <v>99</v>
       </c>
       <c r="Y14" t="s">
         <v>100</v>
@@ -1875,11 +1947,14 @@
       <c r="AA14" t="s">
         <v>100</v>
       </c>
-      <c r="AC14">
+      <c r="AB14" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1920,13 +1995,13 @@
         <v>-82.074333383290821</v>
       </c>
       <c r="N15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O15">
         <v>82.681815410767115</v>
       </c>
       <c r="P15">
-        <v>37.561442077008508</v>
+        <v>50.08490147753767</v>
       </c>
       <c r="Q15">
         <v>82.681815410767115</v>
@@ -1946,8 +2021,8 @@
       <c r="V15">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X15" t="s">
-        <v>100</v>
+      <c r="W15" t="s">
+        <v>99</v>
       </c>
       <c r="Y15" t="s">
         <v>100</v>
@@ -1958,11 +2033,14 @@
       <c r="AA15" t="s">
         <v>100</v>
       </c>
-      <c r="AC15">
+      <c r="AB15" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2003,13 +2081,13 @@
         <v>-90.989975063141983</v>
       </c>
       <c r="N16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O16">
         <v>93.73832830746187</v>
       </c>
       <c r="P16">
-        <v>42.584294643557449</v>
+        <v>56.782436556623132</v>
       </c>
       <c r="Q16">
         <v>93.73832830746187</v>
@@ -2029,8 +2107,8 @@
       <c r="V16">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X16" t="s">
-        <v>100</v>
+      <c r="W16" t="s">
+        <v>99</v>
       </c>
       <c r="Y16" t="s">
         <v>100</v>
@@ -2041,11 +2119,14 @@
       <c r="AA16" t="s">
         <v>100</v>
       </c>
-      <c r="AC16">
+      <c r="AB16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -2086,13 +2167,13 @@
         <v>-347.87434646533711</v>
       </c>
       <c r="N17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O17">
         <v>262.30599999999998</v>
       </c>
       <c r="P17">
-        <v>119.1627394307159</v>
+        <v>158.8931024518383</v>
       </c>
       <c r="Q17">
         <v>262.30599999999998</v>
@@ -2112,8 +2193,8 @@
       <c r="V17">
         <v>0.32269800017361622</v>
       </c>
-      <c r="X17" t="s">
-        <v>100</v>
+      <c r="W17" t="s">
+        <v>99</v>
       </c>
       <c r="Y17" t="s">
         <v>100</v>
@@ -2124,11 +2205,14 @@
       <c r="AA17" t="s">
         <v>100</v>
       </c>
-      <c r="AC17">
+      <c r="AB17" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -2169,13 +2253,13 @@
         <v>-127.014822106826</v>
       </c>
       <c r="N18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O18">
         <v>125.5849553915687</v>
       </c>
       <c r="P18">
-        <v>57.05186810726245</v>
+        <v>76.073681819867105</v>
       </c>
       <c r="Q18">
         <v>125.5849553915687</v>
@@ -2195,8 +2279,8 @@
       <c r="V18">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X18" t="s">
-        <v>100</v>
+      <c r="W18" t="s">
+        <v>99</v>
       </c>
       <c r="Y18" t="s">
         <v>100</v>
@@ -2207,11 +2291,14 @@
       <c r="AA18" t="s">
         <v>100</v>
       </c>
-      <c r="AC18">
+      <c r="AB18" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -2252,13 +2339,13 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O19">
         <v>307.82600000000002</v>
       </c>
       <c r="P19">
-        <v>139.841976271986</v>
+        <v>186.46705815093651</v>
       </c>
       <c r="Q19">
         <v>307.82600000000002</v>
@@ -2278,8 +2365,8 @@
       <c r="V19">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X19" t="s">
-        <v>100</v>
+      <c r="W19" t="s">
+        <v>99</v>
       </c>
       <c r="Y19" t="s">
         <v>100</v>
@@ -2290,11 +2377,14 @@
       <c r="AA19" t="s">
         <v>100</v>
       </c>
-      <c r="AC19">
+      <c r="AB19" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -2335,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -2361,8 +2451,8 @@
       <c r="V20">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X20" t="s">
-        <v>100</v>
+      <c r="W20" t="s">
+        <v>99</v>
       </c>
       <c r="Y20" t="s">
         <v>100</v>
@@ -2373,11 +2463,14 @@
       <c r="AA20" t="s">
         <v>100</v>
       </c>
-      <c r="AC20">
+      <c r="AB20" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2418,13 +2511,13 @@
         <v>20088.831165078151</v>
       </c>
       <c r="N21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O21">
         <v>132998.85200000001</v>
       </c>
       <c r="P21">
-        <v>60419.920037896023</v>
+        <v>80564.684821593386</v>
       </c>
       <c r="Q21">
         <v>132998.85200000001</v>
@@ -2444,23 +2537,26 @@
       <c r="V21">
         <v>-0.21407213503510669</v>
       </c>
-      <c r="X21" t="s">
+      <c r="W21" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y21" t="s">
         <v>101</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>102</v>
       </c>
-      <c r="Z21" t="b">
+      <c r="AA21" t="b">
         <v>1</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="AB21" t="s">
         <v>103</v>
       </c>
-      <c r="AC21">
+      <c r="AD21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -2501,13 +2597,13 @@
         <v>6218.3061853621484</v>
       </c>
       <c r="N22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O22">
         <v>50908.668000000012</v>
       </c>
       <c r="P22">
-        <v>23127.249623145592</v>
+        <v>30838.166874606832</v>
       </c>
       <c r="Q22">
         <v>50908.668000000012</v>
@@ -2527,23 +2623,26 @@
       <c r="V22">
         <v>-0.1849665973728743</v>
       </c>
-      <c r="X22" t="s">
+      <c r="W22" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y22" t="s">
         <v>101</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>102</v>
       </c>
-      <c r="Z22" t="b">
+      <c r="AA22" t="b">
         <v>1</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AB22" t="s">
         <v>103</v>
       </c>
-      <c r="AC22">
+      <c r="AD22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -2584,13 +2683,13 @@
         <v>7256.5882203088186</v>
       </c>
       <c r="N23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O23">
         <v>28154.166000000001</v>
       </c>
       <c r="P23">
-        <v>12790.128883621121</v>
+        <v>17054.519464610268</v>
       </c>
       <c r="Q23">
         <v>28154.166000000001</v>
@@ -2610,23 +2709,26 @@
       <c r="V23">
         <v>-0.32617160708110171</v>
       </c>
-      <c r="X23" t="s">
+      <c r="W23" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y23" t="s">
         <v>101</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Z23" t="s">
         <v>102</v>
       </c>
-      <c r="Z23" t="b">
+      <c r="AA23" t="b">
         <v>1</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="AB23" t="s">
         <v>103</v>
       </c>
-      <c r="AC23">
+      <c r="AD23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2667,13 +2769,13 @@
         <v>2103.5325948250161</v>
       </c>
       <c r="N24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O24">
         <v>7952.3440000000001</v>
       </c>
       <c r="P24">
-        <v>3612.6626761698831</v>
+        <v>4817.1700606324712</v>
       </c>
       <c r="Q24">
         <v>7952.3440000000001</v>
@@ -2693,23 +2795,26 @@
       <c r="V24">
         <v>-0.36063886315653748</v>
       </c>
-      <c r="X24" t="s">
+      <c r="W24" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y24" t="s">
         <v>101</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>102</v>
       </c>
-      <c r="Z24" t="b">
+      <c r="AA24" t="b">
         <v>1</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AB24" t="s">
         <v>103</v>
       </c>
-      <c r="AC24">
+      <c r="AD24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -2750,13 +2855,13 @@
         <v>1832.5284292669489</v>
       </c>
       <c r="N25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O25">
         <v>9813.98</v>
       </c>
       <c r="P25">
-        <v>4458.3834968253013</v>
+        <v>5944.8648891001021</v>
       </c>
       <c r="Q25">
         <v>9813.98</v>
@@ -2776,23 +2881,26 @@
       <c r="V25">
         <v>-0.2377187377531248</v>
       </c>
-      <c r="X25" t="s">
+      <c r="W25" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y25" t="s">
         <v>101</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Z25" t="s">
         <v>102</v>
       </c>
-      <c r="Z25" t="b">
+      <c r="AA25" t="b">
         <v>1</v>
       </c>
-      <c r="AA25" t="s">
+      <c r="AB25" t="s">
         <v>103</v>
       </c>
-      <c r="AC25">
+      <c r="AD25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2833,13 +2941,13 @@
         <v>1251.4957694145801</v>
       </c>
       <c r="N26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O26">
         <v>9631.8079999999991</v>
       </c>
       <c r="P26">
-        <v>4375.6247548690653</v>
+        <v>5834.5133368677616</v>
       </c>
       <c r="Q26">
         <v>9631.8079999999991</v>
@@ -2859,23 +2967,26 @@
       <c r="V26">
         <v>-0.19257211752092471</v>
       </c>
-      <c r="X26" t="s">
+      <c r="W26" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y26" t="s">
         <v>101</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="Z26" t="s">
         <v>102</v>
       </c>
-      <c r="Z26" t="b">
+      <c r="AA26" t="b">
         <v>1</v>
       </c>
-      <c r="AA26" t="s">
+      <c r="AB26" t="s">
         <v>103</v>
       </c>
-      <c r="AC26">
+      <c r="AD26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2916,13 +3027,13 @@
         <v>306.65952663774812</v>
       </c>
       <c r="N27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O27">
         <v>17586.763999999999</v>
       </c>
       <c r="P27">
-        <v>7989.4740339965356</v>
+        <v>10653.265628877351</v>
       </c>
       <c r="Q27">
         <v>17586.763999999999</v>
@@ -2942,23 +3053,26 @@
       <c r="V27">
         <v>-8.0866551329161609E-2</v>
       </c>
-      <c r="X27" t="s">
+      <c r="W27" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y27" t="s">
         <v>101</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>102</v>
       </c>
-      <c r="Z27" t="b">
+      <c r="AA27" t="b">
         <v>1</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AB27" t="s">
         <v>103</v>
       </c>
-      <c r="AC27">
+      <c r="AD27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -2999,13 +3113,13 @@
         <v>979.98142752579952</v>
       </c>
       <c r="N28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O28">
         <v>6186.0820000000003</v>
       </c>
       <c r="P28">
-        <v>2810.2692178716538</v>
+        <v>3747.248484599942</v>
       </c>
       <c r="Q28">
         <v>6186.0820000000003</v>
@@ -3025,23 +3139,26 @@
       <c r="V28">
         <v>-0.1885334420671306</v>
       </c>
-      <c r="X28" t="s">
+      <c r="W28" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y28" t="s">
         <v>101</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="Z28" t="s">
         <v>102</v>
       </c>
-      <c r="Z28" t="b">
+      <c r="AA28" t="b">
         <v>1</v>
       </c>
-      <c r="AA28" t="s">
+      <c r="AB28" t="s">
         <v>103</v>
       </c>
-      <c r="AC28">
+      <c r="AD28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -3082,13 +3199,13 @@
         <v>414.25608649473543</v>
       </c>
       <c r="N29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O29">
         <v>1281.2239999999999</v>
       </c>
       <c r="P29">
-        <v>582.04601368012766</v>
+        <v>776.10750915249355</v>
       </c>
       <c r="Q29">
         <v>1281.2239999999999</v>
@@ -3108,23 +3225,26 @@
       <c r="V29">
         <v>-0.65361718390822532</v>
       </c>
-      <c r="X29" t="s">
+      <c r="W29" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y29" t="s">
         <v>101</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="Z29" t="s">
         <v>102</v>
       </c>
-      <c r="Z29" t="b">
+      <c r="AA29" t="b">
         <v>1</v>
       </c>
-      <c r="AA29" t="s">
+      <c r="AB29" t="s">
         <v>103</v>
       </c>
-      <c r="AC29">
+      <c r="AD29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -3165,13 +3285,13 @@
         <v>500.35636444925098</v>
       </c>
       <c r="N30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O30">
         <v>2220.75</v>
       </c>
       <c r="P30">
-        <v>1008.862372918509</v>
+        <v>1345.2298356496599</v>
       </c>
       <c r="Q30">
         <v>2220.75</v>
@@ -3191,23 +3311,26 @@
       <c r="V30">
         <v>-0.27803279653388191</v>
       </c>
-      <c r="X30" t="s">
+      <c r="W30" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y30" t="s">
         <v>101</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="Z30" t="s">
         <v>102</v>
       </c>
-      <c r="Z30" t="b">
+      <c r="AA30" t="b">
         <v>1</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="AB30" t="s">
         <v>103</v>
       </c>
-      <c r="AC30">
+      <c r="AD30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -3248,13 +3371,13 @@
         <v>283.16743614442572</v>
       </c>
       <c r="N31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O31">
         <v>6271.8559999999989</v>
       </c>
       <c r="P31">
-        <v>2849.2354054995772</v>
+        <v>3799.2064915448991</v>
       </c>
       <c r="Q31">
         <v>6271.8559999999989</v>
@@ -3274,26 +3397,29 @@
       <c r="V31">
         <v>-5.7865465509342663E-2</v>
       </c>
-      <c r="X31" t="s">
+      <c r="W31" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y31" t="s">
         <v>101</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Z31" t="s">
         <v>102</v>
       </c>
-      <c r="Z31" t="b">
+      <c r="AA31" t="b">
         <v>1</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="AB31" t="s">
         <v>103</v>
       </c>
-      <c r="AB31" t="s">
+      <c r="AC31" t="s">
         <v>105</v>
       </c>
-      <c r="AC31">
+      <c r="AD31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -3334,13 +3460,13 @@
         <v>130.87178835850139</v>
       </c>
       <c r="N32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O32">
         <v>3365.45</v>
       </c>
       <c r="P32">
-        <v>1528.887030480061</v>
+        <v>2038.637284875447</v>
       </c>
       <c r="Q32">
         <v>3365.45</v>
@@ -3360,23 +3486,26 @@
       <c r="V32">
         <v>-6.0855415974171552E-2</v>
       </c>
-      <c r="X32" t="s">
+      <c r="W32" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y32" t="s">
         <v>101</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>102</v>
       </c>
-      <c r="Z32" t="b">
+      <c r="AA32" t="b">
         <v>1</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AB32" t="s">
         <v>103</v>
       </c>
-      <c r="AC32">
+      <c r="AD32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -3417,13 +3546,13 @@
         <v>-344.89787125297238</v>
       </c>
       <c r="N33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O33">
         <v>3764.1179999999999</v>
       </c>
       <c r="P33">
-        <v>1709.9975312057959</v>
+        <v>2280.132314986346</v>
       </c>
       <c r="Q33">
         <v>3764.1179999999999</v>
@@ -3443,23 +3572,26 @@
       <c r="V33">
         <v>-5.3425629441463708E-2</v>
       </c>
-      <c r="X33" t="s">
+      <c r="W33" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y33" t="s">
         <v>101</v>
       </c>
-      <c r="Y33" t="s">
+      <c r="Z33" t="s">
         <v>102</v>
       </c>
-      <c r="Z33" t="b">
+      <c r="AA33" t="b">
         <v>1</v>
       </c>
-      <c r="AA33" t="s">
+      <c r="AB33" t="s">
         <v>103</v>
       </c>
-      <c r="AC33">
+      <c r="AD33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -3500,13 +3632,13 @@
         <v>84.204935760502053</v>
       </c>
       <c r="N34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O34">
         <v>850.22800000000007</v>
       </c>
       <c r="P34">
-        <v>386.24925705358908</v>
+        <v>515.02963985353563</v>
       </c>
       <c r="Q34">
         <v>850.22800000000007</v>
@@ -3526,23 +3658,26 @@
       <c r="V34">
         <v>-9.872598710029129E-2</v>
       </c>
-      <c r="X34" t="s">
+      <c r="W34" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y34" t="s">
         <v>101</v>
       </c>
-      <c r="Y34" t="s">
+      <c r="Z34" t="s">
         <v>102</v>
       </c>
-      <c r="Z34" t="b">
+      <c r="AA34" t="b">
         <v>1</v>
       </c>
-      <c r="AA34" t="s">
+      <c r="AB34" t="s">
         <v>103</v>
       </c>
-      <c r="AC34">
+      <c r="AD34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>62</v>
       </c>
@@ -3583,13 +3718,13 @@
         <v>13.11019587385181</v>
       </c>
       <c r="N35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O35">
         <v>3007.7539999999999</v>
       </c>
       <c r="P35">
-        <v>1366.389660067606</v>
+        <v>1821.9612379126911</v>
       </c>
       <c r="Q35">
         <v>3007.7539999999999</v>
@@ -3609,23 +3744,26 @@
       <c r="V35">
         <v>-4.8103319828525486E-3</v>
       </c>
-      <c r="X35" t="s">
+      <c r="W35" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y35" t="s">
         <v>101</v>
       </c>
-      <c r="Y35" t="s">
+      <c r="Z35" t="s">
         <v>102</v>
       </c>
-      <c r="Z35" t="b">
+      <c r="AA35" t="b">
         <v>1</v>
       </c>
-      <c r="AA35" t="s">
+      <c r="AB35" t="s">
         <v>103</v>
       </c>
-      <c r="AC35">
+      <c r="AD35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -3666,13 +3804,13 @@
         <v>-18.836861650014502</v>
       </c>
       <c r="N36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O36">
         <v>1268.296</v>
       </c>
       <c r="P36">
-        <v>576.17296504471597</v>
+        <v>768.27631189243323</v>
       </c>
       <c r="Q36">
         <v>1268.296</v>
@@ -3692,23 +3830,26 @@
       <c r="V36">
         <v>-6.4460581809559934E-3</v>
       </c>
-      <c r="X36" t="s">
+      <c r="W36" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y36" t="s">
         <v>101</v>
       </c>
-      <c r="Y36" t="s">
+      <c r="Z36" t="s">
         <v>102</v>
       </c>
-      <c r="Z36" t="b">
+      <c r="AA36" t="b">
         <v>1</v>
       </c>
-      <c r="AA36" t="s">
+      <c r="AB36" t="s">
         <v>103</v>
       </c>
-      <c r="AC36">
+      <c r="AD36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -3749,13 +3890,13 @@
         <v>981.33560599460134</v>
       </c>
       <c r="N37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O37">
         <v>3019.98</v>
       </c>
       <c r="P37">
-        <v>1371.943797800941</v>
+        <v>1829.367195346284</v>
       </c>
       <c r="Q37">
         <v>3019.98</v>
@@ -3775,23 +3916,26 @@
       <c r="V37">
         <v>-7.2988558937087583E-2</v>
       </c>
-      <c r="X37" t="s">
+      <c r="W37" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y37" t="s">
         <v>101</v>
       </c>
-      <c r="Y37" t="s">
+      <c r="Z37" t="s">
         <v>102</v>
       </c>
-      <c r="Z37" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA37" t="s">
+      <c r="AA37" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB37" t="s">
         <v>104</v>
       </c>
-      <c r="AC37">
+      <c r="AD37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -3832,13 +3976,13 @@
         <v>235.72744935168609</v>
       </c>
       <c r="N38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O38">
         <v>4266.7619999999997</v>
       </c>
       <c r="P38">
-        <v>1938.343188561757</v>
+        <v>2584.6112997934101</v>
       </c>
       <c r="Q38">
         <v>4266.7619999999997</v>
@@ -3858,23 +4002,26 @@
       <c r="V38">
         <v>-4.8284421851105257E-2</v>
       </c>
-      <c r="X38" t="s">
+      <c r="W38" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y38" t="s">
         <v>101</v>
       </c>
-      <c r="Y38" t="s">
+      <c r="Z38" t="s">
         <v>102</v>
       </c>
-      <c r="Z38" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA38" t="s">
+      <c r="AA38" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB38" t="s">
         <v>104</v>
       </c>
-      <c r="AC38">
+      <c r="AD38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -3915,13 +4062,13 @@
         <v>-92.386789961771456</v>
       </c>
       <c r="N39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O39">
         <v>575.74199999999996</v>
       </c>
       <c r="P39">
-        <v>261.55327718511683</v>
+        <v>348.7584446860775</v>
       </c>
       <c r="Q39">
         <v>575.74199999999996</v>
@@ -3941,23 +4088,26 @@
       <c r="V39">
         <v>-4.5966556944716928E-2</v>
       </c>
-      <c r="X39" t="s">
+      <c r="W39" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y39" t="s">
         <v>101</v>
       </c>
-      <c r="Y39" t="s">
+      <c r="Z39" t="s">
         <v>102</v>
       </c>
-      <c r="Z39" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA39" t="s">
+      <c r="AA39" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB39" t="s">
         <v>104</v>
       </c>
-      <c r="AC39">
+      <c r="AD39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -3998,13 +4148,13 @@
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O40">
         <v>500</v>
       </c>
       <c r="P40">
-        <v>227.14451714927591</v>
+        <v>302.87736927832037</v>
       </c>
       <c r="Q40">
         <v>500</v>
@@ -4024,23 +4174,26 @@
       <c r="V40">
         <v>0</v>
       </c>
-      <c r="X40" t="s">
+      <c r="W40" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y40" t="s">
         <v>101</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="Z40" t="s">
         <v>102</v>
       </c>
-      <c r="Z40" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA40" t="s">
+      <c r="AA40" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB40" t="s">
         <v>104</v>
       </c>
-      <c r="AC40">
+      <c r="AD40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -4081,13 +4234,13 @@
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O41">
         <v>5673.94</v>
       </c>
       <c r="P41">
-        <v>2577.6087232679251</v>
+        <v>3437.016041286066</v>
       </c>
       <c r="Q41">
         <v>5673.94</v>
@@ -4107,23 +4260,26 @@
       <c r="V41">
         <v>0</v>
       </c>
-      <c r="X41" t="s">
+      <c r="W41" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y41" t="s">
         <v>101</v>
       </c>
-      <c r="Y41" t="s">
+      <c r="Z41" t="s">
         <v>102</v>
       </c>
-      <c r="Z41" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA41" t="s">
+      <c r="AA41" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB41" t="s">
         <v>104</v>
       </c>
-      <c r="AC41">
+      <c r="AD41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -4164,13 +4320,13 @@
         <v>-7.6211099817555805E-2</v>
       </c>
       <c r="N42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O42">
         <v>2165.4</v>
       </c>
       <c r="P42">
-        <v>983.71747487008406</v>
+        <v>1311.7013108705501</v>
       </c>
       <c r="Q42">
         <v>2165.4</v>
@@ -4190,23 +4346,26 @@
       <c r="V42">
         <v>5.477616236888173E-4</v>
       </c>
-      <c r="X42" t="s">
+      <c r="W42" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y42" t="s">
         <v>101</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="Z42" t="s">
         <v>102</v>
       </c>
-      <c r="Z42" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA42" t="s">
+      <c r="AA42" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB42" t="s">
         <v>104</v>
       </c>
-      <c r="AC42">
+      <c r="AD42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -4247,13 +4406,13 @@
         <v>-290.90583651243969</v>
       </c>
       <c r="N43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O43">
         <v>1291.566</v>
       </c>
       <c r="P43">
-        <v>586.74427087284334</v>
+        <v>782.37222465864647</v>
       </c>
       <c r="Q43">
         <v>1291.566</v>
@@ -4273,23 +4432,26 @@
       <c r="V43">
         <v>1.626468134636078E-2</v>
       </c>
-      <c r="X43" t="s">
+      <c r="W43" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y43" t="s">
         <v>101</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="Z43" t="s">
         <v>102</v>
       </c>
-      <c r="Z43" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA43" t="s">
+      <c r="AA43" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB43" t="s">
         <v>104</v>
       </c>
-      <c r="AC43">
+      <c r="AD43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -4330,13 +4492,13 @@
         <v>-26.107856121190029</v>
       </c>
       <c r="N44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O44">
         <v>1422.87</v>
       </c>
       <c r="P44">
-        <v>646.3942382323803</v>
+        <v>861.91024485008757</v>
       </c>
       <c r="Q44">
         <v>1422.87</v>
@@ -4356,23 +4518,26 @@
       <c r="V44">
         <v>1.510143749118237E-2</v>
       </c>
-      <c r="X44" t="s">
+      <c r="W44" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y44" t="s">
         <v>101</v>
       </c>
-      <c r="Y44" t="s">
+      <c r="Z44" t="s">
         <v>102</v>
       </c>
-      <c r="Z44" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA44" t="s">
+      <c r="AA44" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB44" t="s">
         <v>104</v>
       </c>
-      <c r="AC44">
+      <c r="AD44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -4413,13 +4578,13 @@
         <v>-492.84192149015962</v>
       </c>
       <c r="N45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O45">
         <v>2723.1239999999998</v>
       </c>
       <c r="P45">
-        <v>1237.085372235209</v>
+        <v>1649.545266677314</v>
       </c>
       <c r="Q45">
         <v>2723.1239999999998</v>
@@ -4439,23 +4604,26 @@
       <c r="V45">
         <v>9.1351555057786627E-3</v>
       </c>
-      <c r="X45" t="s">
+      <c r="W45" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y45" t="s">
         <v>101</v>
       </c>
-      <c r="Y45" t="s">
+      <c r="Z45" t="s">
         <v>102</v>
       </c>
-      <c r="Z45" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA45" t="s">
+      <c r="AA45" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB45" t="s">
         <v>104</v>
       </c>
-      <c r="AC45">
+      <c r="AD45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -4496,13 +4664,13 @@
         <v>-93.379452668870726</v>
       </c>
       <c r="N46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O46">
         <v>2568.058</v>
       </c>
       <c r="P46">
-        <v>1166.64058884267</v>
+        <v>1555.6133023882901</v>
       </c>
       <c r="Q46">
         <v>2568.058</v>
@@ -4522,23 +4690,26 @@
       <c r="V46">
         <v>2.1969381420102251E-2</v>
       </c>
-      <c r="X46" t="s">
+      <c r="W46" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y46" t="s">
         <v>101</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="Z46" t="s">
         <v>102</v>
       </c>
-      <c r="Z46" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA46" t="s">
+      <c r="AA46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB46" t="s">
         <v>104</v>
       </c>
-      <c r="AC46">
+      <c r="AD46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -4579,13 +4750,13 @@
         <v>-65.048432230097774</v>
       </c>
       <c r="N47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O47">
         <v>981.74575637584269</v>
       </c>
       <c r="P47">
-        <v>445.99633159068293</v>
+        <v>594.69714398254018</v>
       </c>
       <c r="Q47">
         <v>981.74575637584269</v>
@@ -4605,23 +4776,26 @@
       <c r="V47">
         <v>8.9294861496229755E-2</v>
       </c>
-      <c r="X47" t="s">
+      <c r="W47" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y47" t="s">
         <v>101</v>
       </c>
-      <c r="Y47" t="s">
+      <c r="Z47" t="s">
         <v>102</v>
       </c>
-      <c r="Z47" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA47" t="s">
+      <c r="AA47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB47" t="s">
         <v>104</v>
       </c>
-      <c r="AC47">
+      <c r="AD47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -4662,13 +4836,13 @@
         <v>-233.24861028273151</v>
       </c>
       <c r="N48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O48">
         <v>12053.773999999999</v>
       </c>
       <c r="P48">
-        <v>5475.8973501129913</v>
+        <v>7301.6307179908335</v>
       </c>
       <c r="Q48">
         <v>12053.773999999999</v>
@@ -4688,23 +4862,26 @@
       <c r="V48">
         <v>9.0384089405118606E-3</v>
       </c>
-      <c r="X48" t="s">
+      <c r="W48" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y48" t="s">
         <v>101</v>
       </c>
-      <c r="Y48" t="s">
+      <c r="Z48" t="s">
         <v>102</v>
       </c>
-      <c r="Z48" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA48" t="s">
+      <c r="AA48" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB48" t="s">
         <v>104</v>
       </c>
-      <c r="AC48">
+      <c r="AD48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -4745,13 +4922,13 @@
         <v>-218.0047971699679</v>
       </c>
       <c r="N49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O49">
         <v>219.32328369903061</v>
       </c>
       <c r="P49">
-        <v>99.636162750819892</v>
+        <v>132.8561183764902</v>
       </c>
       <c r="Q49">
         <v>219.32328369903061</v>
@@ -4771,23 +4948,26 @@
       <c r="V49">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X49" t="s">
+      <c r="W49" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y49" t="s">
         <v>101</v>
       </c>
-      <c r="Y49" t="s">
+      <c r="Z49" t="s">
         <v>102</v>
       </c>
-      <c r="Z49" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA49" t="s">
-        <v>100</v>
-      </c>
-      <c r="AC49">
+      <c r="AA49" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -4828,13 +5008,13 @@
         <v>-806.53165411470968</v>
       </c>
       <c r="N50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O50">
         <v>1325</v>
       </c>
       <c r="P50">
-        <v>601.93297044558108</v>
+        <v>802.6250285875492</v>
       </c>
       <c r="Q50">
         <v>1325</v>
@@ -4854,23 +5034,26 @@
       <c r="V50">
         <v>0.17046719495833021</v>
       </c>
-      <c r="X50" t="s">
+      <c r="W50" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y50" t="s">
         <v>101</v>
       </c>
-      <c r="Y50" t="s">
+      <c r="Z50" t="s">
         <v>102</v>
       </c>
-      <c r="Z50" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA50" t="s">
+      <c r="AA50" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB50" t="s">
         <v>104</v>
       </c>
-      <c r="AC50">
+      <c r="AD50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -4911,13 +5094,13 @@
         <v>-275.09702670229598</v>
       </c>
       <c r="N51" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O51">
         <v>773.38</v>
       </c>
       <c r="P51">
-        <v>351.33805334581399</v>
+        <v>468.47859970493488</v>
       </c>
       <c r="Q51">
         <v>773.38</v>
@@ -4937,23 +5120,26 @@
       <c r="V51">
         <v>0.30920198828558337</v>
       </c>
-      <c r="X51" t="s">
+      <c r="W51" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y51" t="s">
         <v>101</v>
       </c>
-      <c r="Y51" t="s">
+      <c r="Z51" t="s">
         <v>102</v>
       </c>
-      <c r="Z51" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA51" t="s">
+      <c r="AA51" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB51" t="s">
         <v>104</v>
       </c>
-      <c r="AC51">
+      <c r="AD51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -4994,13 +5180,13 @@
         <v>-275.09702670229598</v>
       </c>
       <c r="N52" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O52">
         <v>773.38</v>
       </c>
       <c r="P52">
-        <v>351.33805334581399</v>
+        <v>468.47859970493488</v>
       </c>
       <c r="Q52">
         <v>773.38</v>
@@ -5020,23 +5206,26 @@
       <c r="V52">
         <v>0.30920198828558337</v>
       </c>
-      <c r="X52" t="s">
+      <c r="W52" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y52" t="s">
         <v>101</v>
       </c>
-      <c r="Y52" t="s">
+      <c r="Z52" t="s">
         <v>102</v>
       </c>
-      <c r="Z52" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA52" t="s">
+      <c r="AA52" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB52" t="s">
         <v>104</v>
       </c>
-      <c r="AC52">
+      <c r="AD52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -5077,13 +5266,13 @@
         <v>281.99210805393022</v>
       </c>
       <c r="N53" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O53">
         <v>2705.9259999999999</v>
       </c>
       <c r="P53">
-        <v>1229.2725094233431</v>
+        <v>1639.127496683617</v>
       </c>
       <c r="Q53">
         <v>2705.9259999999999</v>
@@ -5103,23 +5292,26 @@
       <c r="V53">
         <v>0.1006627317627756</v>
       </c>
-      <c r="X53" t="s">
+      <c r="W53" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y53" t="s">
         <v>101</v>
       </c>
-      <c r="Y53" t="s">
+      <c r="Z53" t="s">
         <v>102</v>
       </c>
-      <c r="Z53" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA53" t="s">
+      <c r="AA53" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB53" t="s">
         <v>104</v>
       </c>
-      <c r="AC53">
+      <c r="AD53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>81</v>
       </c>
@@ -5160,13 +5352,13 @@
         <v>-615.66295275155244</v>
       </c>
       <c r="N54" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O54">
         <v>9796.8320000000003</v>
       </c>
       <c r="P54">
-        <v>4450.5933484651496</v>
+        <v>5934.4774068433326</v>
       </c>
       <c r="Q54">
         <v>9796.8320000000003</v>
@@ -5186,23 +5378,26 @@
       <c r="V54">
         <v>2.9652511711154479E-2</v>
       </c>
-      <c r="X54" t="s">
+      <c r="W54" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y54" t="s">
         <v>101</v>
       </c>
-      <c r="Y54" t="s">
+      <c r="Z54" t="s">
         <v>102</v>
       </c>
-      <c r="Z54" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA54" t="s">
+      <c r="AA54" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB54" t="s">
         <v>104</v>
       </c>
-      <c r="AC54">
+      <c r="AD54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -5243,13 +5438,13 @@
         <v>-1215.905209574297</v>
       </c>
       <c r="N55" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O55">
         <v>5344.93</v>
       </c>
       <c r="P55">
-        <v>2428.143088093359</v>
+        <v>3237.7166747535471</v>
       </c>
       <c r="Q55">
         <v>5344.93</v>
@@ -5269,23 +5464,26 @@
       <c r="V55">
         <v>6.0203868911808678E-2</v>
       </c>
-      <c r="X55" t="s">
+      <c r="W55" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y55" t="s">
         <v>101</v>
       </c>
-      <c r="Y55" t="s">
+      <c r="Z55" t="s">
         <v>102</v>
       </c>
-      <c r="Z55" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA55" t="s">
+      <c r="AA55" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB55" t="s">
         <v>104</v>
       </c>
-      <c r="AC55">
+      <c r="AD55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -5326,13 +5524,13 @@
         <v>-337.55129314181801</v>
       </c>
       <c r="N56" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O56">
         <v>2911.19</v>
       </c>
       <c r="P56">
-        <v>1322.521693759601</v>
+        <v>1763.4671373387071</v>
       </c>
       <c r="Q56">
         <v>2911.19</v>
@@ -5352,26 +5550,29 @@
       <c r="V56">
         <v>0.1139530401640691</v>
       </c>
-      <c r="X56" t="s">
+      <c r="W56" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y56" t="s">
         <v>101</v>
       </c>
-      <c r="Y56" t="s">
+      <c r="Z56" t="s">
         <v>102</v>
       </c>
-      <c r="Z56" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA56" t="s">
+      <c r="AA56" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB56" t="s">
         <v>104</v>
       </c>
-      <c r="AB56" t="s">
+      <c r="AC56" t="s">
         <v>105</v>
       </c>
-      <c r="AC56">
+      <c r="AD56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>84</v>
       </c>
@@ -5412,13 +5613,13 @@
         <v>-2506.0205875146689</v>
       </c>
       <c r="N57" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O57">
         <v>3530.5</v>
       </c>
       <c r="P57">
-        <v>1603.8674355910371</v>
+        <v>2138.61710447422</v>
       </c>
       <c r="Q57">
         <v>3530.5</v>
@@ -5438,23 +5639,26 @@
       <c r="V57">
         <v>0.2060831065824183</v>
       </c>
-      <c r="X57" t="s">
+      <c r="W57" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y57" t="s">
         <v>101</v>
       </c>
-      <c r="Y57" t="s">
+      <c r="Z57" t="s">
         <v>102</v>
       </c>
-      <c r="Z57" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA57" t="s">
+      <c r="AA57" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB57" t="s">
         <v>104</v>
       </c>
-      <c r="AC57">
+      <c r="AD57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>85</v>
       </c>
@@ -5495,13 +5699,13 @@
         <v>-1601.2318775221081</v>
       </c>
       <c r="N58" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O58">
         <v>14092.082</v>
       </c>
       <c r="P58">
-        <v>6401.8783230360041</v>
+        <v>8536.3454476287443</v>
       </c>
       <c r="Q58">
         <v>14092.082</v>
@@ -5521,23 +5725,26 @@
       <c r="V58">
         <v>7.0503908655811298E-2</v>
       </c>
-      <c r="X58" t="s">
+      <c r="W58" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y58" t="s">
         <v>101</v>
       </c>
-      <c r="Y58" t="s">
+      <c r="Z58" t="s">
         <v>102</v>
       </c>
-      <c r="Z58" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA58" t="s">
+      <c r="AA58" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB58" t="s">
         <v>104</v>
       </c>
-      <c r="AC58">
+      <c r="AD58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -5578,13 +5785,13 @@
         <v>-1658.5766880363869</v>
       </c>
       <c r="N59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O59">
         <v>8073.7160000000003</v>
       </c>
       <c r="P59">
-        <v>3667.8006448407659</v>
+        <v>4890.6917247605688</v>
       </c>
       <c r="Q59">
         <v>8073.7160000000003</v>
@@ -5604,23 +5811,26 @@
       <c r="V59">
         <v>0.12765603647889351</v>
       </c>
-      <c r="X59" t="s">
+      <c r="W59" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y59" t="s">
         <v>101</v>
       </c>
-      <c r="Y59" t="s">
+      <c r="Z59" t="s">
         <v>102</v>
       </c>
-      <c r="Z59" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA59" t="s">
+      <c r="AA59" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB59" t="s">
         <v>104</v>
       </c>
-      <c r="AC59">
+      <c r="AD59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -5661,13 +5871,13 @@
         <v>-3381.5925902386348</v>
       </c>
       <c r="N60" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O60">
         <v>10719.157999999999</v>
       </c>
       <c r="P60">
-        <v>4869.5959363135953</v>
+        <v>6493.1807518373253</v>
       </c>
       <c r="Q60">
         <v>10719.157999999999</v>
@@ -5687,23 +5897,26 @@
       <c r="V60">
         <v>0.10095157399245171</v>
       </c>
-      <c r="X60" t="s">
+      <c r="W60" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y60" t="s">
         <v>101</v>
       </c>
-      <c r="Y60" t="s">
+      <c r="Z60" t="s">
         <v>102</v>
       </c>
-      <c r="Z60" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA60" t="s">
+      <c r="AA60" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB60" t="s">
         <v>104</v>
       </c>
-      <c r="AC60">
+      <c r="AD60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -5744,13 +5957,13 @@
         <v>-6043.6799597968857</v>
       </c>
       <c r="N61" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O61">
         <v>8559.8040000000001</v>
       </c>
       <c r="P61">
-        <v>3888.6250929448811</v>
+        <v>5185.1418341160888</v>
       </c>
       <c r="Q61">
         <v>8559.8040000000001</v>
@@ -5770,23 +5983,26 @@
       <c r="V61">
         <v>0.16467129399024941</v>
       </c>
-      <c r="X61" t="s">
+      <c r="W61" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y61" t="s">
         <v>101</v>
       </c>
-      <c r="Y61" t="s">
+      <c r="Z61" t="s">
         <v>102</v>
       </c>
-      <c r="Z61" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA61" t="s">
+      <c r="AA61" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB61" t="s">
         <v>104</v>
       </c>
-      <c r="AC61">
+      <c r="AD61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>89</v>
       </c>
@@ -5827,13 +6043,13 @@
         <v>201.79142876003701</v>
       </c>
       <c r="N62" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O62">
         <v>925.67506422228098</v>
       </c>
       <c r="P62">
-        <v>420.52403099978989</v>
+        <v>560.73205651636954</v>
       </c>
       <c r="Q62">
         <v>925.67506422228098</v>
@@ -5853,23 +6069,26 @@
       <c r="V62">
         <v>0.30790533512762669</v>
       </c>
-      <c r="X62" t="s">
+      <c r="W62" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y62" t="s">
         <v>101</v>
       </c>
-      <c r="Y62" t="s">
+      <c r="Z62" t="s">
         <v>102</v>
       </c>
-      <c r="Z62" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA62" t="s">
+      <c r="AA62" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB62" t="s">
         <v>104</v>
       </c>
-      <c r="AC62">
+      <c r="AD62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -5910,13 +6129,13 @@
         <v>-1134.449821186477</v>
       </c>
       <c r="N63" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O63">
         <v>35431.038967668093</v>
       </c>
       <c r="P63">
-        <v>16095.932476816301</v>
+        <v>21462.519746649941</v>
       </c>
       <c r="Q63">
         <v>35431.038967668093</v>
@@ -5936,23 +6155,26 @@
       <c r="V63">
         <v>5.1821897353325791E-2</v>
       </c>
-      <c r="X63" t="s">
+      <c r="W63" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y63" t="s">
         <v>101</v>
       </c>
-      <c r="Y63" t="s">
+      <c r="Z63" t="s">
         <v>102</v>
       </c>
-      <c r="Z63" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA63" t="s">
+      <c r="AA63" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB63" t="s">
         <v>104</v>
       </c>
-      <c r="AC63">
+      <c r="AD63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>91</v>
       </c>
@@ -5993,13 +6215,13 @@
         <v>-2025.330851793537</v>
       </c>
       <c r="N64" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O64">
         <v>17467.126</v>
       </c>
       <c r="P64">
-        <v>7935.1238025111252</v>
+        <v>10580.794343465899</v>
       </c>
       <c r="Q64">
         <v>17467.126</v>
@@ -6019,23 +6241,26 @@
       <c r="V64">
         <v>0.11395352837981609</v>
       </c>
-      <c r="X64" t="s">
+      <c r="W64" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y64" t="s">
         <v>101</v>
       </c>
-      <c r="Y64" t="s">
+      <c r="Z64" t="s">
         <v>102</v>
       </c>
-      <c r="Z64" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA64" t="s">
+      <c r="AA64" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB64" t="s">
         <v>104</v>
       </c>
-      <c r="AC64">
+      <c r="AD64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>92</v>
       </c>
@@ -6076,13 +6301,13 @@
         <v>-675.77502354874377</v>
       </c>
       <c r="N65" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O65">
         <v>17906.646532179231</v>
       </c>
       <c r="P65">
-        <v>8134.7931606292123</v>
+        <v>10847.03598852641</v>
       </c>
       <c r="Q65">
         <v>17906.646532179231</v>
@@ -6102,23 +6327,26 @@
       <c r="V65">
         <v>9.7796498291219197E-2</v>
       </c>
-      <c r="X65" t="s">
+      <c r="W65" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y65" t="s">
         <v>101</v>
       </c>
-      <c r="Y65" t="s">
+      <c r="Z65" t="s">
         <v>102</v>
       </c>
-      <c r="Z65" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA65" t="s">
+      <c r="AA65" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB65" t="s">
         <v>104</v>
       </c>
-      <c r="AC65">
+      <c r="AD65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>93</v>
       </c>
@@ -6159,13 +6387,13 @@
         <v>-1372.023218097409</v>
       </c>
       <c r="N66" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O66">
         <v>13927.162781718391</v>
       </c>
       <c r="P66">
-        <v>6326.9573306255779</v>
+        <v>8436.4448496756013</v>
       </c>
       <c r="Q66">
         <v>13927.162781718391</v>
@@ -6185,186 +6413,23 @@
       <c r="V66">
         <v>0.13528927757787881</v>
       </c>
-      <c r="X66" t="s">
+      <c r="W66" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y66" t="s">
         <v>101</v>
       </c>
-      <c r="Y66" t="s">
+      <c r="Z66" t="s">
         <v>102</v>
       </c>
-      <c r="Z66" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA66" t="s">
+      <c r="AA66" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB66" t="s">
         <v>104</v>
       </c>
-      <c r="AC66">
+      <c r="AD66">
         <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>94</v>
-      </c>
-      <c r="B67">
-        <v>259261.53</v>
-      </c>
-      <c r="C67">
-        <v>346507.55</v>
-      </c>
-      <c r="D67">
-        <v>310339.83</v>
-      </c>
-      <c r="E67">
-        <v>270786.08</v>
-      </c>
-      <c r="F67">
-        <v>224941.28</v>
-      </c>
-      <c r="G67">
-        <v>5</v>
-      </c>
-      <c r="H67" t="b">
-        <v>0</v>
-      </c>
-      <c r="I67">
-        <v>0.69069999999999998</v>
-      </c>
-      <c r="J67">
-        <v>267231.13267906482</v>
-      </c>
-      <c r="K67">
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="L67">
-        <v>0</v>
-      </c>
-      <c r="M67">
-        <v>4517.2220049124153</v>
-      </c>
-      <c r="N67" t="s">
-        <v>98</v>
-      </c>
-      <c r="O67">
-        <v>220420.74290606481</v>
-      </c>
-      <c r="P67">
-        <v>100134.7264341655</v>
-      </c>
-      <c r="Q67">
-        <v>220420.74290606481</v>
-      </c>
-      <c r="R67">
-        <v>296723.74749999988</v>
-      </c>
-      <c r="S67">
-        <v>282367.25400000002</v>
-      </c>
-      <c r="T67">
-        <v>-71782.467499999941</v>
-      </c>
-      <c r="U67">
-        <v>-0.2419168270311764</v>
-      </c>
-      <c r="V67">
-        <v>9.5674208367960131E-2</v>
-      </c>
-      <c r="X67" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y67" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z67" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA67" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC67">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>95</v>
-      </c>
-      <c r="B68">
-        <v>22.77</v>
-      </c>
-      <c r="C68">
-        <v>115787.2</v>
-      </c>
-      <c r="D68">
-        <v>65210.11</v>
-      </c>
-      <c r="E68">
-        <v>18382.03</v>
-      </c>
-      <c r="F68">
-        <v>-63098.82</v>
-      </c>
-      <c r="G68">
-        <v>5</v>
-      </c>
-      <c r="H68" t="b">
-        <v>0</v>
-      </c>
-      <c r="I68">
-        <v>0.99390000000000001</v>
-      </c>
-      <c r="J68">
-        <v>5477.9922713783963</v>
-      </c>
-      <c r="K68">
-        <v>0.998</v>
-      </c>
-      <c r="L68">
-        <v>0</v>
-      </c>
-      <c r="M68">
-        <v>-1215.905209574295</v>
-      </c>
-      <c r="N68" t="s">
-        <v>98</v>
-      </c>
-      <c r="O68">
-        <v>-61880.986149621611</v>
-      </c>
-      <c r="P68">
-        <v>-28111.853439353661</v>
-      </c>
-      <c r="Q68">
-        <v>-61880.986149621611</v>
-      </c>
-      <c r="R68">
-        <v>49850.527499999997</v>
-      </c>
-      <c r="S68">
-        <v>27260.657999999999</v>
-      </c>
-      <c r="T68">
-        <v>-112949.3475</v>
-      </c>
-      <c r="U68">
-        <v>-2.2657603272101778</v>
-      </c>
-      <c r="V68">
-        <v>0.89607171323153911</v>
-      </c>
-      <c r="X68" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y68" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z68" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA68" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC68">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update index.html and commit current expense-analysis.xlsx before pulling remote changes
</commit_message>
<xml_diff>
--- a/public/expense-analysis.xlsx
+++ b/public/expense-analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/Library/Mobile Documents/com~apple~CloudDocs/Gilliam/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-gilliam-roanoke-1/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1DC99B0-09AA-CC40-9B0B-75DF59A55B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7D48C3-2420-6544-8C2F-E55C1748CC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="20120" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="107">
   <si>
     <t>Category</t>
   </si>
@@ -304,12 +304,6 @@
     <t>Medical Supplies</t>
   </si>
   <si>
-    <t>Gross Profit</t>
-  </si>
-  <si>
-    <t>Net Ordinary Income</t>
-  </si>
-  <si>
     <t>Clamped</t>
   </si>
   <si>
@@ -322,6 +316,12 @@
     <t>One-time</t>
   </si>
   <si>
+    <t>Costs Declined Despite Profit Growth</t>
+  </si>
+  <si>
+    <t>Costs Grew Slower than Profit</t>
+  </si>
+  <si>
     <t>Below Threshold</t>
   </si>
   <si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Under-Leveraged</t>
+  </si>
+  <si>
+    <t>Expense Growth Alignment</t>
   </si>
 </sst>
 </file>
@@ -705,13 +708,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC68"/>
+  <dimension ref="A1:AD66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -779,28 +812,31 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -841,13 +877,13 @@
         <v>1053.8418543645289</v>
       </c>
       <c r="N2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O2">
         <v>626.65200000000004</v>
       </c>
       <c r="P2">
-        <v>284.68113192125611</v>
+        <v>379.59741842599612</v>
       </c>
       <c r="Q2">
         <v>626.65200000000004</v>
@@ -867,8 +903,8 @@
       <c r="V2">
         <v>-125.7704011981041</v>
       </c>
-      <c r="X2" t="s">
-        <v>100</v>
+      <c r="W2" t="s">
+        <v>98</v>
       </c>
       <c r="Y2" t="s">
         <v>100</v>
@@ -877,13 +913,16 @@
         <v>100</v>
       </c>
       <c r="AA2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB2" t="s">
         <v>103</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -924,13 +963,13 @@
         <v>1053.8418543645289</v>
       </c>
       <c r="N3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O3">
         <v>626.65200000000004</v>
       </c>
       <c r="P3">
-        <v>284.68113192125611</v>
+        <v>379.59741842599612</v>
       </c>
       <c r="Q3">
         <v>626.65200000000004</v>
@@ -950,8 +989,8 @@
       <c r="V3">
         <v>-125.7704011981041</v>
       </c>
-      <c r="X3" t="s">
-        <v>100</v>
+      <c r="W3" t="s">
+        <v>98</v>
       </c>
       <c r="Y3" t="s">
         <v>100</v>
@@ -960,13 +999,16 @@
         <v>100</v>
       </c>
       <c r="AA3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB3" t="s">
         <v>103</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1007,13 +1049,13 @@
         <v>1215.905209574297</v>
       </c>
       <c r="N4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O4">
         <v>-5344.93</v>
       </c>
       <c r="P4">
-        <v>-2428.143088093359</v>
+        <v>-3237.7166747535471</v>
       </c>
       <c r="Q4">
         <v>-5344.93</v>
@@ -1033,8 +1075,8 @@
       <c r="V4">
         <v>6.0203868911808678E-2</v>
       </c>
-      <c r="X4" t="s">
-        <v>100</v>
+      <c r="W4" t="s">
+        <v>99</v>
       </c>
       <c r="Y4" t="s">
         <v>100</v>
@@ -1045,11 +1087,14 @@
       <c r="AA4" t="s">
         <v>100</v>
       </c>
-      <c r="AC4">
+      <c r="AB4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1090,13 +1135,13 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O5">
         <v>493.75200000000012</v>
       </c>
       <c r="P5">
-        <v>224.3061192629786</v>
+        <v>299.09261367181858</v>
       </c>
       <c r="Q5">
         <v>493.75200000000012</v>
@@ -1116,8 +1161,8 @@
       <c r="V5">
         <v>-0.45404564609826009</v>
       </c>
-      <c r="X5" t="s">
-        <v>100</v>
+      <c r="W5" t="s">
+        <v>98</v>
       </c>
       <c r="Y5" t="s">
         <v>100</v>
@@ -1128,11 +1173,14 @@
       <c r="AA5" t="s">
         <v>100</v>
       </c>
-      <c r="AC5">
+      <c r="AB5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1173,13 +1221,13 @@
         <v>-12.743006246802681</v>
       </c>
       <c r="N6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O6">
         <v>281.98399999999998</v>
       </c>
       <c r="P6">
-        <v>128.10223904764291</v>
+        <v>170.81314419715591</v>
       </c>
       <c r="Q6">
         <v>281.98399999999998</v>
@@ -1199,8 +1247,8 @@
       <c r="V6">
         <v>-0.58190788706878993</v>
       </c>
-      <c r="X6" t="s">
-        <v>100</v>
+      <c r="W6" t="s">
+        <v>98</v>
       </c>
       <c r="Y6" t="s">
         <v>100</v>
@@ -1211,11 +1259,14 @@
       <c r="AA6" t="s">
         <v>100</v>
       </c>
-      <c r="AC6">
+      <c r="AB6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1256,13 +1307,13 @@
         <v>60.235031218222097</v>
       </c>
       <c r="N7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O7">
         <v>104.79600000000001</v>
       </c>
       <c r="P7">
-        <v>47.607673638351038</v>
+        <v>63.480673581781737</v>
       </c>
       <c r="Q7">
         <v>104.79600000000001</v>
@@ -1282,8 +1333,8 @@
       <c r="V7">
         <v>-1.210177060389181</v>
       </c>
-      <c r="X7" t="s">
-        <v>100</v>
+      <c r="W7" t="s">
+        <v>98</v>
       </c>
       <c r="Y7" t="s">
         <v>100</v>
@@ -1294,11 +1345,14 @@
       <c r="AA7" t="s">
         <v>100</v>
       </c>
-      <c r="AC7">
+      <c r="AB7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1339,13 +1393,13 @@
         <v>57.344810514279857</v>
       </c>
       <c r="N8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O8">
         <v>344.42599999999999</v>
       </c>
       <c r="P8">
-        <v>156.46895492731301</v>
+        <v>208.63768158210959</v>
       </c>
       <c r="Q8">
         <v>344.42599999999999</v>
@@ -1365,8 +1419,8 @@
       <c r="V8">
         <v>-0.231961024274254</v>
       </c>
-      <c r="X8" t="s">
-        <v>100</v>
+      <c r="W8" t="s">
+        <v>98</v>
       </c>
       <c r="Y8" t="s">
         <v>100</v>
@@ -1377,11 +1431,14 @@
       <c r="AA8" t="s">
         <v>100</v>
       </c>
-      <c r="AC8">
+      <c r="AB8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1422,13 +1479,13 @@
         <v>84.31720770385266</v>
       </c>
       <c r="N9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O9">
         <v>381.00599999999997</v>
       </c>
       <c r="P9">
-        <v>173.08684780195401</v>
+        <v>230.79618991851149</v>
       </c>
       <c r="Q9">
         <v>381.00599999999997</v>
@@ -1448,8 +1505,8 @@
       <c r="V9">
         <v>-7.0067423191985963E-5</v>
       </c>
-      <c r="X9" t="s">
-        <v>100</v>
+      <c r="W9" t="s">
+        <v>98</v>
       </c>
       <c r="Y9" t="s">
         <v>100</v>
@@ -1460,11 +1517,14 @@
       <c r="AA9" t="s">
         <v>100</v>
       </c>
-      <c r="AC9">
+      <c r="AB9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1505,13 +1565,13 @@
         <v>-0.204142920372373</v>
       </c>
       <c r="N10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O10">
         <v>5.9100445581432153</v>
       </c>
       <c r="P10">
-        <v>2.684868434980292</v>
+        <v>3.580037496176141</v>
       </c>
       <c r="Q10">
         <v>5.9100445581432153</v>
@@ -1531,8 +1591,8 @@
       <c r="V10">
         <v>0.1318279641011087</v>
       </c>
-      <c r="X10" t="s">
-        <v>100</v>
+      <c r="W10" t="s">
+        <v>99</v>
       </c>
       <c r="Y10" t="s">
         <v>100</v>
@@ -1543,11 +1603,14 @@
       <c r="AA10" t="s">
         <v>100</v>
       </c>
-      <c r="AC10">
+      <c r="AB10" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1588,13 +1651,13 @@
         <v>-24.563487227989999</v>
       </c>
       <c r="N11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O11">
         <v>100.70399999999999</v>
       </c>
       <c r="P11">
-        <v>45.748722910001362</v>
+        <v>61.00192519160796</v>
       </c>
       <c r="Q11">
         <v>100.70399999999999</v>
@@ -1614,8 +1677,8 @@
       <c r="V11">
         <v>7.9820362483175575E-2</v>
       </c>
-      <c r="X11" t="s">
-        <v>100</v>
+      <c r="W11" t="s">
+        <v>99</v>
       </c>
       <c r="Y11" t="s">
         <v>100</v>
@@ -1626,11 +1689,14 @@
       <c r="AA11" t="s">
         <v>100</v>
       </c>
-      <c r="AC11">
+      <c r="AB11" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1671,13 +1737,13 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O12">
         <v>32.770000000000003</v>
       </c>
       <c r="P12">
-        <v>14.887051653963541</v>
+        <v>19.850582782501121</v>
       </c>
       <c r="Q12">
         <v>32.770000000000003</v>
@@ -1697,8 +1763,8 @@
       <c r="V12">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X12" t="s">
-        <v>100</v>
+      <c r="W12" t="s">
+        <v>99</v>
       </c>
       <c r="Y12" t="s">
         <v>100</v>
@@ -1709,11 +1775,14 @@
       <c r="AA12" t="s">
         <v>100</v>
       </c>
-      <c r="AC12">
+      <c r="AB12" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1754,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -1780,8 +1849,8 @@
       <c r="V13">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X13" t="s">
-        <v>100</v>
+      <c r="W13" t="s">
+        <v>99</v>
       </c>
       <c r="Y13" t="s">
         <v>100</v>
@@ -1792,11 +1861,14 @@
       <c r="AA13" t="s">
         <v>100</v>
       </c>
-      <c r="AC13">
+      <c r="AB13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1837,13 +1909,13 @@
         <v>5.7030506926241458</v>
       </c>
       <c r="N14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O14">
         <v>-7.8874317955383484</v>
       </c>
       <c r="P14">
-        <v>-3.5831737734908078</v>
+        <v>-4.7778491851896678</v>
       </c>
       <c r="Q14">
         <v>-7.8874317955383484</v>
@@ -1863,8 +1935,8 @@
       <c r="V14">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X14" t="s">
-        <v>100</v>
+      <c r="W14" t="s">
+        <v>99</v>
       </c>
       <c r="Y14" t="s">
         <v>100</v>
@@ -1875,11 +1947,14 @@
       <c r="AA14" t="s">
         <v>100</v>
       </c>
-      <c r="AC14">
+      <c r="AB14" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1920,13 +1995,13 @@
         <v>-82.074333383290821</v>
       </c>
       <c r="N15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O15">
         <v>82.681815410767115</v>
       </c>
       <c r="P15">
-        <v>37.561442077008508</v>
+        <v>50.08490147753767</v>
       </c>
       <c r="Q15">
         <v>82.681815410767115</v>
@@ -1946,8 +2021,8 @@
       <c r="V15">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X15" t="s">
-        <v>100</v>
+      <c r="W15" t="s">
+        <v>99</v>
       </c>
       <c r="Y15" t="s">
         <v>100</v>
@@ -1958,11 +2033,14 @@
       <c r="AA15" t="s">
         <v>100</v>
       </c>
-      <c r="AC15">
+      <c r="AB15" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2003,13 +2081,13 @@
         <v>-90.989975063141983</v>
       </c>
       <c r="N16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O16">
         <v>93.73832830746187</v>
       </c>
       <c r="P16">
-        <v>42.584294643557449</v>
+        <v>56.782436556623132</v>
       </c>
       <c r="Q16">
         <v>93.73832830746187</v>
@@ -2029,8 +2107,8 @@
       <c r="V16">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X16" t="s">
-        <v>100</v>
+      <c r="W16" t="s">
+        <v>99</v>
       </c>
       <c r="Y16" t="s">
         <v>100</v>
@@ -2041,11 +2119,14 @@
       <c r="AA16" t="s">
         <v>100</v>
       </c>
-      <c r="AC16">
+      <c r="AB16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -2086,13 +2167,13 @@
         <v>-347.87434646533711</v>
       </c>
       <c r="N17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O17">
         <v>262.30599999999998</v>
       </c>
       <c r="P17">
-        <v>119.1627394307159</v>
+        <v>158.8931024518383</v>
       </c>
       <c r="Q17">
         <v>262.30599999999998</v>
@@ -2112,8 +2193,8 @@
       <c r="V17">
         <v>0.32269800017361622</v>
       </c>
-      <c r="X17" t="s">
-        <v>100</v>
+      <c r="W17" t="s">
+        <v>99</v>
       </c>
       <c r="Y17" t="s">
         <v>100</v>
@@ -2124,11 +2205,14 @@
       <c r="AA17" t="s">
         <v>100</v>
       </c>
-      <c r="AC17">
+      <c r="AB17" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -2169,13 +2253,13 @@
         <v>-127.014822106826</v>
       </c>
       <c r="N18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O18">
         <v>125.5849553915687</v>
       </c>
       <c r="P18">
-        <v>57.05186810726245</v>
+        <v>76.073681819867105</v>
       </c>
       <c r="Q18">
         <v>125.5849553915687</v>
@@ -2195,8 +2279,8 @@
       <c r="V18">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X18" t="s">
-        <v>100</v>
+      <c r="W18" t="s">
+        <v>99</v>
       </c>
       <c r="Y18" t="s">
         <v>100</v>
@@ -2207,11 +2291,14 @@
       <c r="AA18" t="s">
         <v>100</v>
       </c>
-      <c r="AC18">
+      <c r="AB18" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -2252,13 +2339,13 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O19">
         <v>307.82600000000002</v>
       </c>
       <c r="P19">
-        <v>139.841976271986</v>
+        <v>186.46705815093651</v>
       </c>
       <c r="Q19">
         <v>307.82600000000002</v>
@@ -2278,8 +2365,8 @@
       <c r="V19">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X19" t="s">
-        <v>100</v>
+      <c r="W19" t="s">
+        <v>99</v>
       </c>
       <c r="Y19" t="s">
         <v>100</v>
@@ -2290,11 +2377,14 @@
       <c r="AA19" t="s">
         <v>100</v>
       </c>
-      <c r="AC19">
+      <c r="AB19" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -2335,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -2361,8 +2451,8 @@
       <c r="V20">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X20" t="s">
-        <v>100</v>
+      <c r="W20" t="s">
+        <v>99</v>
       </c>
       <c r="Y20" t="s">
         <v>100</v>
@@ -2373,11 +2463,14 @@
       <c r="AA20" t="s">
         <v>100</v>
       </c>
-      <c r="AC20">
+      <c r="AB20" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2418,13 +2511,13 @@
         <v>20088.831165078151</v>
       </c>
       <c r="N21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O21">
         <v>132998.85200000001</v>
       </c>
       <c r="P21">
-        <v>60419.920037896023</v>
+        <v>80564.684821593386</v>
       </c>
       <c r="Q21">
         <v>132998.85200000001</v>
@@ -2444,23 +2537,26 @@
       <c r="V21">
         <v>-0.21407213503510669</v>
       </c>
-      <c r="X21" t="s">
+      <c r="W21" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y21" t="s">
         <v>101</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>102</v>
       </c>
-      <c r="Z21" t="b">
+      <c r="AA21" t="b">
         <v>1</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="AB21" t="s">
         <v>103</v>
       </c>
-      <c r="AC21">
+      <c r="AD21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -2501,13 +2597,13 @@
         <v>6218.3061853621484</v>
       </c>
       <c r="N22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O22">
         <v>50908.668000000012</v>
       </c>
       <c r="P22">
-        <v>23127.249623145592</v>
+        <v>30838.166874606832</v>
       </c>
       <c r="Q22">
         <v>50908.668000000012</v>
@@ -2527,23 +2623,26 @@
       <c r="V22">
         <v>-0.1849665973728743</v>
       </c>
-      <c r="X22" t="s">
+      <c r="W22" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y22" t="s">
         <v>101</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>102</v>
       </c>
-      <c r="Z22" t="b">
+      <c r="AA22" t="b">
         <v>1</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AB22" t="s">
         <v>103</v>
       </c>
-      <c r="AC22">
+      <c r="AD22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -2584,13 +2683,13 @@
         <v>7256.5882203088186</v>
       </c>
       <c r="N23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O23">
         <v>28154.166000000001</v>
       </c>
       <c r="P23">
-        <v>12790.128883621121</v>
+        <v>17054.519464610268</v>
       </c>
       <c r="Q23">
         <v>28154.166000000001</v>
@@ -2610,23 +2709,26 @@
       <c r="V23">
         <v>-0.32617160708110171</v>
       </c>
-      <c r="X23" t="s">
+      <c r="W23" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y23" t="s">
         <v>101</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Z23" t="s">
         <v>102</v>
       </c>
-      <c r="Z23" t="b">
+      <c r="AA23" t="b">
         <v>1</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="AB23" t="s">
         <v>103</v>
       </c>
-      <c r="AC23">
+      <c r="AD23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2667,13 +2769,13 @@
         <v>2103.5325948250161</v>
       </c>
       <c r="N24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O24">
         <v>7952.3440000000001</v>
       </c>
       <c r="P24">
-        <v>3612.6626761698831</v>
+        <v>4817.1700606324712</v>
       </c>
       <c r="Q24">
         <v>7952.3440000000001</v>
@@ -2693,23 +2795,26 @@
       <c r="V24">
         <v>-0.36063886315653748</v>
       </c>
-      <c r="X24" t="s">
+      <c r="W24" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y24" t="s">
         <v>101</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>102</v>
       </c>
-      <c r="Z24" t="b">
+      <c r="AA24" t="b">
         <v>1</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AB24" t="s">
         <v>103</v>
       </c>
-      <c r="AC24">
+      <c r="AD24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -2750,13 +2855,13 @@
         <v>1832.5284292669489</v>
       </c>
       <c r="N25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O25">
         <v>9813.98</v>
       </c>
       <c r="P25">
-        <v>4458.3834968253013</v>
+        <v>5944.8648891001021</v>
       </c>
       <c r="Q25">
         <v>9813.98</v>
@@ -2776,23 +2881,26 @@
       <c r="V25">
         <v>-0.2377187377531248</v>
       </c>
-      <c r="X25" t="s">
+      <c r="W25" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y25" t="s">
         <v>101</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Z25" t="s">
         <v>102</v>
       </c>
-      <c r="Z25" t="b">
+      <c r="AA25" t="b">
         <v>1</v>
       </c>
-      <c r="AA25" t="s">
+      <c r="AB25" t="s">
         <v>103</v>
       </c>
-      <c r="AC25">
+      <c r="AD25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2833,13 +2941,13 @@
         <v>1251.4957694145801</v>
       </c>
       <c r="N26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O26">
         <v>9631.8079999999991</v>
       </c>
       <c r="P26">
-        <v>4375.6247548690653</v>
+        <v>5834.5133368677616</v>
       </c>
       <c r="Q26">
         <v>9631.8079999999991</v>
@@ -2859,23 +2967,26 @@
       <c r="V26">
         <v>-0.19257211752092471</v>
       </c>
-      <c r="X26" t="s">
+      <c r="W26" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y26" t="s">
         <v>101</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="Z26" t="s">
         <v>102</v>
       </c>
-      <c r="Z26" t="b">
+      <c r="AA26" t="b">
         <v>1</v>
       </c>
-      <c r="AA26" t="s">
+      <c r="AB26" t="s">
         <v>103</v>
       </c>
-      <c r="AC26">
+      <c r="AD26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2916,13 +3027,13 @@
         <v>306.65952663774812</v>
       </c>
       <c r="N27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O27">
         <v>17586.763999999999</v>
       </c>
       <c r="P27">
-        <v>7989.4740339965356</v>
+        <v>10653.265628877351</v>
       </c>
       <c r="Q27">
         <v>17586.763999999999</v>
@@ -2942,23 +3053,26 @@
       <c r="V27">
         <v>-8.0866551329161609E-2</v>
       </c>
-      <c r="X27" t="s">
+      <c r="W27" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y27" t="s">
         <v>101</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>102</v>
       </c>
-      <c r="Z27" t="b">
+      <c r="AA27" t="b">
         <v>1</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AB27" t="s">
         <v>103</v>
       </c>
-      <c r="AC27">
+      <c r="AD27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -2999,13 +3113,13 @@
         <v>979.98142752579952</v>
       </c>
       <c r="N28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O28">
         <v>6186.0820000000003</v>
       </c>
       <c r="P28">
-        <v>2810.2692178716538</v>
+        <v>3747.248484599942</v>
       </c>
       <c r="Q28">
         <v>6186.0820000000003</v>
@@ -3025,23 +3139,26 @@
       <c r="V28">
         <v>-0.1885334420671306</v>
       </c>
-      <c r="X28" t="s">
+      <c r="W28" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y28" t="s">
         <v>101</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="Z28" t="s">
         <v>102</v>
       </c>
-      <c r="Z28" t="b">
+      <c r="AA28" t="b">
         <v>1</v>
       </c>
-      <c r="AA28" t="s">
+      <c r="AB28" t="s">
         <v>103</v>
       </c>
-      <c r="AC28">
+      <c r="AD28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -3082,13 +3199,13 @@
         <v>414.25608649473543</v>
       </c>
       <c r="N29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O29">
         <v>1281.2239999999999</v>
       </c>
       <c r="P29">
-        <v>582.04601368012766</v>
+        <v>776.10750915249355</v>
       </c>
       <c r="Q29">
         <v>1281.2239999999999</v>
@@ -3108,23 +3225,26 @@
       <c r="V29">
         <v>-0.65361718390822532</v>
       </c>
-      <c r="X29" t="s">
+      <c r="W29" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y29" t="s">
         <v>101</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="Z29" t="s">
         <v>102</v>
       </c>
-      <c r="Z29" t="b">
+      <c r="AA29" t="b">
         <v>1</v>
       </c>
-      <c r="AA29" t="s">
+      <c r="AB29" t="s">
         <v>103</v>
       </c>
-      <c r="AC29">
+      <c r="AD29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -3165,13 +3285,13 @@
         <v>500.35636444925098</v>
       </c>
       <c r="N30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O30">
         <v>2220.75</v>
       </c>
       <c r="P30">
-        <v>1008.862372918509</v>
+        <v>1345.2298356496599</v>
       </c>
       <c r="Q30">
         <v>2220.75</v>
@@ -3191,23 +3311,26 @@
       <c r="V30">
         <v>-0.27803279653388191</v>
       </c>
-      <c r="X30" t="s">
+      <c r="W30" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y30" t="s">
         <v>101</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="Z30" t="s">
         <v>102</v>
       </c>
-      <c r="Z30" t="b">
+      <c r="AA30" t="b">
         <v>1</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="AB30" t="s">
         <v>103</v>
       </c>
-      <c r="AC30">
+      <c r="AD30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -3248,13 +3371,13 @@
         <v>283.16743614442572</v>
       </c>
       <c r="N31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O31">
         <v>6271.8559999999989</v>
       </c>
       <c r="P31">
-        <v>2849.2354054995772</v>
+        <v>3799.2064915448991</v>
       </c>
       <c r="Q31">
         <v>6271.8559999999989</v>
@@ -3274,26 +3397,29 @@
       <c r="V31">
         <v>-5.7865465509342663E-2</v>
       </c>
-      <c r="X31" t="s">
+      <c r="W31" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y31" t="s">
         <v>101</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Z31" t="s">
         <v>102</v>
       </c>
-      <c r="Z31" t="b">
+      <c r="AA31" t="b">
         <v>1</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="AB31" t="s">
         <v>103</v>
       </c>
-      <c r="AB31" t="s">
+      <c r="AC31" t="s">
         <v>105</v>
       </c>
-      <c r="AC31">
+      <c r="AD31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -3334,13 +3460,13 @@
         <v>130.87178835850139</v>
       </c>
       <c r="N32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O32">
         <v>3365.45</v>
       </c>
       <c r="P32">
-        <v>1528.887030480061</v>
+        <v>2038.637284875447</v>
       </c>
       <c r="Q32">
         <v>3365.45</v>
@@ -3360,23 +3486,26 @@
       <c r="V32">
         <v>-6.0855415974171552E-2</v>
       </c>
-      <c r="X32" t="s">
+      <c r="W32" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y32" t="s">
         <v>101</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>102</v>
       </c>
-      <c r="Z32" t="b">
+      <c r="AA32" t="b">
         <v>1</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AB32" t="s">
         <v>103</v>
       </c>
-      <c r="AC32">
+      <c r="AD32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -3417,13 +3546,13 @@
         <v>-344.89787125297238</v>
       </c>
       <c r="N33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O33">
         <v>3764.1179999999999</v>
       </c>
       <c r="P33">
-        <v>1709.9975312057959</v>
+        <v>2280.132314986346</v>
       </c>
       <c r="Q33">
         <v>3764.1179999999999</v>
@@ -3443,23 +3572,26 @@
       <c r="V33">
         <v>-5.3425629441463708E-2</v>
       </c>
-      <c r="X33" t="s">
+      <c r="W33" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y33" t="s">
         <v>101</v>
       </c>
-      <c r="Y33" t="s">
+      <c r="Z33" t="s">
         <v>102</v>
       </c>
-      <c r="Z33" t="b">
+      <c r="AA33" t="b">
         <v>1</v>
       </c>
-      <c r="AA33" t="s">
+      <c r="AB33" t="s">
         <v>103</v>
       </c>
-      <c r="AC33">
+      <c r="AD33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -3500,13 +3632,13 @@
         <v>84.204935760502053</v>
       </c>
       <c r="N34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O34">
         <v>850.22800000000007</v>
       </c>
       <c r="P34">
-        <v>386.24925705358908</v>
+        <v>515.02963985353563</v>
       </c>
       <c r="Q34">
         <v>850.22800000000007</v>
@@ -3526,23 +3658,26 @@
       <c r="V34">
         <v>-9.872598710029129E-2</v>
       </c>
-      <c r="X34" t="s">
+      <c r="W34" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y34" t="s">
         <v>101</v>
       </c>
-      <c r="Y34" t="s">
+      <c r="Z34" t="s">
         <v>102</v>
       </c>
-      <c r="Z34" t="b">
+      <c r="AA34" t="b">
         <v>1</v>
       </c>
-      <c r="AA34" t="s">
+      <c r="AB34" t="s">
         <v>103</v>
       </c>
-      <c r="AC34">
+      <c r="AD34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>62</v>
       </c>
@@ -3583,13 +3718,13 @@
         <v>13.11019587385181</v>
       </c>
       <c r="N35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O35">
         <v>3007.7539999999999</v>
       </c>
       <c r="P35">
-        <v>1366.389660067606</v>
+        <v>1821.9612379126911</v>
       </c>
       <c r="Q35">
         <v>3007.7539999999999</v>
@@ -3609,23 +3744,26 @@
       <c r="V35">
         <v>-4.8103319828525486E-3</v>
       </c>
-      <c r="X35" t="s">
+      <c r="W35" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y35" t="s">
         <v>101</v>
       </c>
-      <c r="Y35" t="s">
+      <c r="Z35" t="s">
         <v>102</v>
       </c>
-      <c r="Z35" t="b">
+      <c r="AA35" t="b">
         <v>1</v>
       </c>
-      <c r="AA35" t="s">
+      <c r="AB35" t="s">
         <v>103</v>
       </c>
-      <c r="AC35">
+      <c r="AD35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -3666,13 +3804,13 @@
         <v>-18.836861650014502</v>
       </c>
       <c r="N36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O36">
         <v>1268.296</v>
       </c>
       <c r="P36">
-        <v>576.17296504471597</v>
+        <v>768.27631189243323</v>
       </c>
       <c r="Q36">
         <v>1268.296</v>
@@ -3692,23 +3830,26 @@
       <c r="V36">
         <v>-6.4460581809559934E-3</v>
       </c>
-      <c r="X36" t="s">
+      <c r="W36" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y36" t="s">
         <v>101</v>
       </c>
-      <c r="Y36" t="s">
+      <c r="Z36" t="s">
         <v>102</v>
       </c>
-      <c r="Z36" t="b">
+      <c r="AA36" t="b">
         <v>1</v>
       </c>
-      <c r="AA36" t="s">
+      <c r="AB36" t="s">
         <v>103</v>
       </c>
-      <c r="AC36">
+      <c r="AD36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -3749,13 +3890,13 @@
         <v>981.33560599460134</v>
       </c>
       <c r="N37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O37">
         <v>3019.98</v>
       </c>
       <c r="P37">
-        <v>1371.943797800941</v>
+        <v>1829.367195346284</v>
       </c>
       <c r="Q37">
         <v>3019.98</v>
@@ -3775,23 +3916,26 @@
       <c r="V37">
         <v>-7.2988558937087583E-2</v>
       </c>
-      <c r="X37" t="s">
+      <c r="W37" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y37" t="s">
         <v>101</v>
       </c>
-      <c r="Y37" t="s">
+      <c r="Z37" t="s">
         <v>102</v>
       </c>
-      <c r="Z37" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA37" t="s">
+      <c r="AA37" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB37" t="s">
         <v>104</v>
       </c>
-      <c r="AC37">
+      <c r="AD37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -3832,13 +3976,13 @@
         <v>235.72744935168609</v>
       </c>
       <c r="N38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O38">
         <v>4266.7619999999997</v>
       </c>
       <c r="P38">
-        <v>1938.343188561757</v>
+        <v>2584.6112997934101</v>
       </c>
       <c r="Q38">
         <v>4266.7619999999997</v>
@@ -3858,23 +4002,26 @@
       <c r="V38">
         <v>-4.8284421851105257E-2</v>
       </c>
-      <c r="X38" t="s">
+      <c r="W38" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y38" t="s">
         <v>101</v>
       </c>
-      <c r="Y38" t="s">
+      <c r="Z38" t="s">
         <v>102</v>
       </c>
-      <c r="Z38" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA38" t="s">
+      <c r="AA38" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB38" t="s">
         <v>104</v>
       </c>
-      <c r="AC38">
+      <c r="AD38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -3915,13 +4062,13 @@
         <v>-92.386789961771456</v>
       </c>
       <c r="N39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O39">
         <v>575.74199999999996</v>
       </c>
       <c r="P39">
-        <v>261.55327718511683</v>
+        <v>348.7584446860775</v>
       </c>
       <c r="Q39">
         <v>575.74199999999996</v>
@@ -3941,23 +4088,26 @@
       <c r="V39">
         <v>-4.5966556944716928E-2</v>
       </c>
-      <c r="X39" t="s">
+      <c r="W39" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y39" t="s">
         <v>101</v>
       </c>
-      <c r="Y39" t="s">
+      <c r="Z39" t="s">
         <v>102</v>
       </c>
-      <c r="Z39" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA39" t="s">
+      <c r="AA39" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB39" t="s">
         <v>104</v>
       </c>
-      <c r="AC39">
+      <c r="AD39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -3998,13 +4148,13 @@
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O40">
         <v>500</v>
       </c>
       <c r="P40">
-        <v>227.14451714927591</v>
+        <v>302.87736927832037</v>
       </c>
       <c r="Q40">
         <v>500</v>
@@ -4024,23 +4174,26 @@
       <c r="V40">
         <v>0</v>
       </c>
-      <c r="X40" t="s">
+      <c r="W40" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y40" t="s">
         <v>101</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="Z40" t="s">
         <v>102</v>
       </c>
-      <c r="Z40" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA40" t="s">
+      <c r="AA40" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB40" t="s">
         <v>104</v>
       </c>
-      <c r="AC40">
+      <c r="AD40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -4081,13 +4234,13 @@
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O41">
         <v>5673.94</v>
       </c>
       <c r="P41">
-        <v>2577.6087232679251</v>
+        <v>3437.016041286066</v>
       </c>
       <c r="Q41">
         <v>5673.94</v>
@@ -4107,23 +4260,26 @@
       <c r="V41">
         <v>0</v>
       </c>
-      <c r="X41" t="s">
+      <c r="W41" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y41" t="s">
         <v>101</v>
       </c>
-      <c r="Y41" t="s">
+      <c r="Z41" t="s">
         <v>102</v>
       </c>
-      <c r="Z41" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA41" t="s">
+      <c r="AA41" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB41" t="s">
         <v>104</v>
       </c>
-      <c r="AC41">
+      <c r="AD41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -4164,13 +4320,13 @@
         <v>-7.6211099817555805E-2</v>
       </c>
       <c r="N42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O42">
         <v>2165.4</v>
       </c>
       <c r="P42">
-        <v>983.71747487008406</v>
+        <v>1311.7013108705501</v>
       </c>
       <c r="Q42">
         <v>2165.4</v>
@@ -4190,23 +4346,26 @@
       <c r="V42">
         <v>5.477616236888173E-4</v>
       </c>
-      <c r="X42" t="s">
+      <c r="W42" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y42" t="s">
         <v>101</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="Z42" t="s">
         <v>102</v>
       </c>
-      <c r="Z42" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA42" t="s">
+      <c r="AA42" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB42" t="s">
         <v>104</v>
       </c>
-      <c r="AC42">
+      <c r="AD42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -4247,13 +4406,13 @@
         <v>-290.90583651243969</v>
       </c>
       <c r="N43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O43">
         <v>1291.566</v>
       </c>
       <c r="P43">
-        <v>586.74427087284334</v>
+        <v>782.37222465864647</v>
       </c>
       <c r="Q43">
         <v>1291.566</v>
@@ -4273,23 +4432,26 @@
       <c r="V43">
         <v>1.626468134636078E-2</v>
       </c>
-      <c r="X43" t="s">
+      <c r="W43" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y43" t="s">
         <v>101</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="Z43" t="s">
         <v>102</v>
       </c>
-      <c r="Z43" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA43" t="s">
+      <c r="AA43" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB43" t="s">
         <v>104</v>
       </c>
-      <c r="AC43">
+      <c r="AD43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -4330,13 +4492,13 @@
         <v>-26.107856121190029</v>
       </c>
       <c r="N44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O44">
         <v>1422.87</v>
       </c>
       <c r="P44">
-        <v>646.3942382323803</v>
+        <v>861.91024485008757</v>
       </c>
       <c r="Q44">
         <v>1422.87</v>
@@ -4356,23 +4518,26 @@
       <c r="V44">
         <v>1.510143749118237E-2</v>
       </c>
-      <c r="X44" t="s">
+      <c r="W44" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y44" t="s">
         <v>101</v>
       </c>
-      <c r="Y44" t="s">
+      <c r="Z44" t="s">
         <v>102</v>
       </c>
-      <c r="Z44" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA44" t="s">
+      <c r="AA44" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB44" t="s">
         <v>104</v>
       </c>
-      <c r="AC44">
+      <c r="AD44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -4413,13 +4578,13 @@
         <v>-492.84192149015962</v>
       </c>
       <c r="N45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O45">
         <v>2723.1239999999998</v>
       </c>
       <c r="P45">
-        <v>1237.085372235209</v>
+        <v>1649.545266677314</v>
       </c>
       <c r="Q45">
         <v>2723.1239999999998</v>
@@ -4439,23 +4604,26 @@
       <c r="V45">
         <v>9.1351555057786627E-3</v>
       </c>
-      <c r="X45" t="s">
+      <c r="W45" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y45" t="s">
         <v>101</v>
       </c>
-      <c r="Y45" t="s">
+      <c r="Z45" t="s">
         <v>102</v>
       </c>
-      <c r="Z45" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA45" t="s">
+      <c r="AA45" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB45" t="s">
         <v>104</v>
       </c>
-      <c r="AC45">
+      <c r="AD45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -4496,13 +4664,13 @@
         <v>-93.379452668870726</v>
       </c>
       <c r="N46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O46">
         <v>2568.058</v>
       </c>
       <c r="P46">
-        <v>1166.64058884267</v>
+        <v>1555.6133023882901</v>
       </c>
       <c r="Q46">
         <v>2568.058</v>
@@ -4522,23 +4690,26 @@
       <c r="V46">
         <v>2.1969381420102251E-2</v>
       </c>
-      <c r="X46" t="s">
+      <c r="W46" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y46" t="s">
         <v>101</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="Z46" t="s">
         <v>102</v>
       </c>
-      <c r="Z46" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA46" t="s">
+      <c r="AA46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB46" t="s">
         <v>104</v>
       </c>
-      <c r="AC46">
+      <c r="AD46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -4579,13 +4750,13 @@
         <v>-65.048432230097774</v>
       </c>
       <c r="N47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O47">
         <v>981.74575637584269</v>
       </c>
       <c r="P47">
-        <v>445.99633159068293</v>
+        <v>594.69714398254018</v>
       </c>
       <c r="Q47">
         <v>981.74575637584269</v>
@@ -4605,23 +4776,26 @@
       <c r="V47">
         <v>8.9294861496229755E-2</v>
       </c>
-      <c r="X47" t="s">
+      <c r="W47" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y47" t="s">
         <v>101</v>
       </c>
-      <c r="Y47" t="s">
+      <c r="Z47" t="s">
         <v>102</v>
       </c>
-      <c r="Z47" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA47" t="s">
+      <c r="AA47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB47" t="s">
         <v>104</v>
       </c>
-      <c r="AC47">
+      <c r="AD47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -4662,13 +4836,13 @@
         <v>-233.24861028273151</v>
       </c>
       <c r="N48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O48">
         <v>12053.773999999999</v>
       </c>
       <c r="P48">
-        <v>5475.8973501129913</v>
+        <v>7301.6307179908335</v>
       </c>
       <c r="Q48">
         <v>12053.773999999999</v>
@@ -4688,23 +4862,26 @@
       <c r="V48">
         <v>9.0384089405118606E-3</v>
       </c>
-      <c r="X48" t="s">
+      <c r="W48" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y48" t="s">
         <v>101</v>
       </c>
-      <c r="Y48" t="s">
+      <c r="Z48" t="s">
         <v>102</v>
       </c>
-      <c r="Z48" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA48" t="s">
+      <c r="AA48" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB48" t="s">
         <v>104</v>
       </c>
-      <c r="AC48">
+      <c r="AD48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -4745,13 +4922,13 @@
         <v>-218.0047971699679</v>
       </c>
       <c r="N49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O49">
         <v>219.32328369903061</v>
       </c>
       <c r="P49">
-        <v>99.636162750819892</v>
+        <v>132.8561183764902</v>
       </c>
       <c r="Q49">
         <v>219.32328369903061</v>
@@ -4771,23 +4948,26 @@
       <c r="V49">
         <v>0.39548389230332609</v>
       </c>
-      <c r="X49" t="s">
+      <c r="W49" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y49" t="s">
         <v>101</v>
       </c>
-      <c r="Y49" t="s">
+      <c r="Z49" t="s">
         <v>102</v>
       </c>
-      <c r="Z49" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA49" t="s">
-        <v>100</v>
-      </c>
-      <c r="AC49">
+      <c r="AA49" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -4828,13 +5008,13 @@
         <v>-806.53165411470968</v>
       </c>
       <c r="N50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O50">
         <v>1325</v>
       </c>
       <c r="P50">
-        <v>601.93297044558108</v>
+        <v>802.6250285875492</v>
       </c>
       <c r="Q50">
         <v>1325</v>
@@ -4854,23 +5034,26 @@
       <c r="V50">
         <v>0.17046719495833021</v>
       </c>
-      <c r="X50" t="s">
+      <c r="W50" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y50" t="s">
         <v>101</v>
       </c>
-      <c r="Y50" t="s">
+      <c r="Z50" t="s">
         <v>102</v>
       </c>
-      <c r="Z50" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA50" t="s">
+      <c r="AA50" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB50" t="s">
         <v>104</v>
       </c>
-      <c r="AC50">
+      <c r="AD50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -4911,13 +5094,13 @@
         <v>-275.09702670229598</v>
       </c>
       <c r="N51" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O51">
         <v>773.38</v>
       </c>
       <c r="P51">
-        <v>351.33805334581399</v>
+        <v>468.47859970493488</v>
       </c>
       <c r="Q51">
         <v>773.38</v>
@@ -4937,23 +5120,26 @@
       <c r="V51">
         <v>0.30920198828558337</v>
       </c>
-      <c r="X51" t="s">
+      <c r="W51" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y51" t="s">
         <v>101</v>
       </c>
-      <c r="Y51" t="s">
+      <c r="Z51" t="s">
         <v>102</v>
       </c>
-      <c r="Z51" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA51" t="s">
+      <c r="AA51" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB51" t="s">
         <v>104</v>
       </c>
-      <c r="AC51">
+      <c r="AD51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -4994,13 +5180,13 @@
         <v>-275.09702670229598</v>
       </c>
       <c r="N52" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O52">
         <v>773.38</v>
       </c>
       <c r="P52">
-        <v>351.33805334581399</v>
+        <v>468.47859970493488</v>
       </c>
       <c r="Q52">
         <v>773.38</v>
@@ -5020,23 +5206,26 @@
       <c r="V52">
         <v>0.30920198828558337</v>
       </c>
-      <c r="X52" t="s">
+      <c r="W52" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y52" t="s">
         <v>101</v>
       </c>
-      <c r="Y52" t="s">
+      <c r="Z52" t="s">
         <v>102</v>
       </c>
-      <c r="Z52" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA52" t="s">
+      <c r="AA52" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB52" t="s">
         <v>104</v>
       </c>
-      <c r="AC52">
+      <c r="AD52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -5077,13 +5266,13 @@
         <v>281.99210805393022</v>
       </c>
       <c r="N53" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O53">
         <v>2705.9259999999999</v>
       </c>
       <c r="P53">
-        <v>1229.2725094233431</v>
+        <v>1639.127496683617</v>
       </c>
       <c r="Q53">
         <v>2705.9259999999999</v>
@@ -5103,23 +5292,26 @@
       <c r="V53">
         <v>0.1006627317627756</v>
       </c>
-      <c r="X53" t="s">
+      <c r="W53" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y53" t="s">
         <v>101</v>
       </c>
-      <c r="Y53" t="s">
+      <c r="Z53" t="s">
         <v>102</v>
       </c>
-      <c r="Z53" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA53" t="s">
+      <c r="AA53" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB53" t="s">
         <v>104</v>
       </c>
-      <c r="AC53">
+      <c r="AD53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>81</v>
       </c>
@@ -5160,13 +5352,13 @@
         <v>-615.66295275155244</v>
       </c>
       <c r="N54" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O54">
         <v>9796.8320000000003</v>
       </c>
       <c r="P54">
-        <v>4450.5933484651496</v>
+        <v>5934.4774068433326</v>
       </c>
       <c r="Q54">
         <v>9796.8320000000003</v>
@@ -5186,23 +5378,26 @@
       <c r="V54">
         <v>2.9652511711154479E-2</v>
       </c>
-      <c r="X54" t="s">
+      <c r="W54" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y54" t="s">
         <v>101</v>
       </c>
-      <c r="Y54" t="s">
+      <c r="Z54" t="s">
         <v>102</v>
       </c>
-      <c r="Z54" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA54" t="s">
+      <c r="AA54" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB54" t="s">
         <v>104</v>
       </c>
-      <c r="AC54">
+      <c r="AD54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -5243,13 +5438,13 @@
         <v>-1215.905209574297</v>
       </c>
       <c r="N55" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O55">
         <v>5344.93</v>
       </c>
       <c r="P55">
-        <v>2428.143088093359</v>
+        <v>3237.7166747535471</v>
       </c>
       <c r="Q55">
         <v>5344.93</v>
@@ -5269,23 +5464,26 @@
       <c r="V55">
         <v>6.0203868911808678E-2</v>
       </c>
-      <c r="X55" t="s">
+      <c r="W55" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y55" t="s">
         <v>101</v>
       </c>
-      <c r="Y55" t="s">
+      <c r="Z55" t="s">
         <v>102</v>
       </c>
-      <c r="Z55" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA55" t="s">
+      <c r="AA55" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB55" t="s">
         <v>104</v>
       </c>
-      <c r="AC55">
+      <c r="AD55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -5326,13 +5524,13 @@
         <v>-337.55129314181801</v>
       </c>
       <c r="N56" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O56">
         <v>2911.19</v>
       </c>
       <c r="P56">
-        <v>1322.521693759601</v>
+        <v>1763.4671373387071</v>
       </c>
       <c r="Q56">
         <v>2911.19</v>
@@ -5352,26 +5550,29 @@
       <c r="V56">
         <v>0.1139530401640691</v>
       </c>
-      <c r="X56" t="s">
+      <c r="W56" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y56" t="s">
         <v>101</v>
       </c>
-      <c r="Y56" t="s">
+      <c r="Z56" t="s">
         <v>102</v>
       </c>
-      <c r="Z56" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA56" t="s">
+      <c r="AA56" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB56" t="s">
         <v>104</v>
       </c>
-      <c r="AB56" t="s">
+      <c r="AC56" t="s">
         <v>105</v>
       </c>
-      <c r="AC56">
+      <c r="AD56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>84</v>
       </c>
@@ -5412,13 +5613,13 @@
         <v>-2506.0205875146689</v>
       </c>
       <c r="N57" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O57">
         <v>3530.5</v>
       </c>
       <c r="P57">
-        <v>1603.8674355910371</v>
+        <v>2138.61710447422</v>
       </c>
       <c r="Q57">
         <v>3530.5</v>
@@ -5438,23 +5639,26 @@
       <c r="V57">
         <v>0.2060831065824183</v>
       </c>
-      <c r="X57" t="s">
+      <c r="W57" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y57" t="s">
         <v>101</v>
       </c>
-      <c r="Y57" t="s">
+      <c r="Z57" t="s">
         <v>102</v>
       </c>
-      <c r="Z57" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA57" t="s">
+      <c r="AA57" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB57" t="s">
         <v>104</v>
       </c>
-      <c r="AC57">
+      <c r="AD57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>85</v>
       </c>
@@ -5495,13 +5699,13 @@
         <v>-1601.2318775221081</v>
       </c>
       <c r="N58" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O58">
         <v>14092.082</v>
       </c>
       <c r="P58">
-        <v>6401.8783230360041</v>
+        <v>8536.3454476287443</v>
       </c>
       <c r="Q58">
         <v>14092.082</v>
@@ -5521,23 +5725,26 @@
       <c r="V58">
         <v>7.0503908655811298E-2</v>
       </c>
-      <c r="X58" t="s">
+      <c r="W58" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y58" t="s">
         <v>101</v>
       </c>
-      <c r="Y58" t="s">
+      <c r="Z58" t="s">
         <v>102</v>
       </c>
-      <c r="Z58" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA58" t="s">
+      <c r="AA58" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB58" t="s">
         <v>104</v>
       </c>
-      <c r="AC58">
+      <c r="AD58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -5578,13 +5785,13 @@
         <v>-1658.5766880363869</v>
       </c>
       <c r="N59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O59">
         <v>8073.7160000000003</v>
       </c>
       <c r="P59">
-        <v>3667.8006448407659</v>
+        <v>4890.6917247605688</v>
       </c>
       <c r="Q59">
         <v>8073.7160000000003</v>
@@ -5604,23 +5811,26 @@
       <c r="V59">
         <v>0.12765603647889351</v>
       </c>
-      <c r="X59" t="s">
+      <c r="W59" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y59" t="s">
         <v>101</v>
       </c>
-      <c r="Y59" t="s">
+      <c r="Z59" t="s">
         <v>102</v>
       </c>
-      <c r="Z59" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA59" t="s">
+      <c r="AA59" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB59" t="s">
         <v>104</v>
       </c>
-      <c r="AC59">
+      <c r="AD59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -5661,13 +5871,13 @@
         <v>-3381.5925902386348</v>
       </c>
       <c r="N60" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O60">
         <v>10719.157999999999</v>
       </c>
       <c r="P60">
-        <v>4869.5959363135953</v>
+        <v>6493.1807518373253</v>
       </c>
       <c r="Q60">
         <v>10719.157999999999</v>
@@ -5687,23 +5897,26 @@
       <c r="V60">
         <v>0.10095157399245171</v>
       </c>
-      <c r="X60" t="s">
+      <c r="W60" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y60" t="s">
         <v>101</v>
       </c>
-      <c r="Y60" t="s">
+      <c r="Z60" t="s">
         <v>102</v>
       </c>
-      <c r="Z60" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA60" t="s">
+      <c r="AA60" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB60" t="s">
         <v>104</v>
       </c>
-      <c r="AC60">
+      <c r="AD60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -5744,13 +5957,13 @@
         <v>-6043.6799597968857</v>
       </c>
       <c r="N61" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O61">
         <v>8559.8040000000001</v>
       </c>
       <c r="P61">
-        <v>3888.6250929448811</v>
+        <v>5185.1418341160888</v>
       </c>
       <c r="Q61">
         <v>8559.8040000000001</v>
@@ -5770,23 +5983,26 @@
       <c r="V61">
         <v>0.16467129399024941</v>
       </c>
-      <c r="X61" t="s">
+      <c r="W61" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y61" t="s">
         <v>101</v>
       </c>
-      <c r="Y61" t="s">
+      <c r="Z61" t="s">
         <v>102</v>
       </c>
-      <c r="Z61" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA61" t="s">
+      <c r="AA61" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB61" t="s">
         <v>104</v>
       </c>
-      <c r="AC61">
+      <c r="AD61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>89</v>
       </c>
@@ -5827,13 +6043,13 @@
         <v>201.79142876003701</v>
       </c>
       <c r="N62" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O62">
         <v>925.67506422228098</v>
       </c>
       <c r="P62">
-        <v>420.52403099978989</v>
+        <v>560.73205651636954</v>
       </c>
       <c r="Q62">
         <v>925.67506422228098</v>
@@ -5853,23 +6069,26 @@
       <c r="V62">
         <v>0.30790533512762669</v>
       </c>
-      <c r="X62" t="s">
+      <c r="W62" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y62" t="s">
         <v>101</v>
       </c>
-      <c r="Y62" t="s">
+      <c r="Z62" t="s">
         <v>102</v>
       </c>
-      <c r="Z62" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA62" t="s">
+      <c r="AA62" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB62" t="s">
         <v>104</v>
       </c>
-      <c r="AC62">
+      <c r="AD62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -5910,13 +6129,13 @@
         <v>-1134.449821186477</v>
       </c>
       <c r="N63" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O63">
         <v>35431.038967668093</v>
       </c>
       <c r="P63">
-        <v>16095.932476816301</v>
+        <v>21462.519746649941</v>
       </c>
       <c r="Q63">
         <v>35431.038967668093</v>
@@ -5936,23 +6155,26 @@
       <c r="V63">
         <v>5.1821897353325791E-2</v>
       </c>
-      <c r="X63" t="s">
+      <c r="W63" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y63" t="s">
         <v>101</v>
       </c>
-      <c r="Y63" t="s">
+      <c r="Z63" t="s">
         <v>102</v>
       </c>
-      <c r="Z63" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA63" t="s">
+      <c r="AA63" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB63" t="s">
         <v>104</v>
       </c>
-      <c r="AC63">
+      <c r="AD63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>91</v>
       </c>
@@ -5993,13 +6215,13 @@
         <v>-2025.330851793537</v>
       </c>
       <c r="N64" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O64">
         <v>17467.126</v>
       </c>
       <c r="P64">
-        <v>7935.1238025111252</v>
+        <v>10580.794343465899</v>
       </c>
       <c r="Q64">
         <v>17467.126</v>
@@ -6019,23 +6241,26 @@
       <c r="V64">
         <v>0.11395352837981609</v>
       </c>
-      <c r="X64" t="s">
+      <c r="W64" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y64" t="s">
         <v>101</v>
       </c>
-      <c r="Y64" t="s">
+      <c r="Z64" t="s">
         <v>102</v>
       </c>
-      <c r="Z64" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA64" t="s">
+      <c r="AA64" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB64" t="s">
         <v>104</v>
       </c>
-      <c r="AC64">
+      <c r="AD64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>92</v>
       </c>
@@ -6076,13 +6301,13 @@
         <v>-675.77502354874377</v>
       </c>
       <c r="N65" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O65">
         <v>17906.646532179231</v>
       </c>
       <c r="P65">
-        <v>8134.7931606292123</v>
+        <v>10847.03598852641</v>
       </c>
       <c r="Q65">
         <v>17906.646532179231</v>
@@ -6102,23 +6327,26 @@
       <c r="V65">
         <v>9.7796498291219197E-2</v>
       </c>
-      <c r="X65" t="s">
+      <c r="W65" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y65" t="s">
         <v>101</v>
       </c>
-      <c r="Y65" t="s">
+      <c r="Z65" t="s">
         <v>102</v>
       </c>
-      <c r="Z65" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA65" t="s">
+      <c r="AA65" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB65" t="s">
         <v>104</v>
       </c>
-      <c r="AC65">
+      <c r="AD65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>93</v>
       </c>
@@ -6159,13 +6387,13 @@
         <v>-1372.023218097409</v>
       </c>
       <c r="N66" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O66">
         <v>13927.162781718391</v>
       </c>
       <c r="P66">
-        <v>6326.9573306255779</v>
+        <v>8436.4448496756013</v>
       </c>
       <c r="Q66">
         <v>13927.162781718391</v>
@@ -6185,186 +6413,23 @@
       <c r="V66">
         <v>0.13528927757787881</v>
       </c>
-      <c r="X66" t="s">
+      <c r="W66" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y66" t="s">
         <v>101</v>
       </c>
-      <c r="Y66" t="s">
+      <c r="Z66" t="s">
         <v>102</v>
       </c>
-      <c r="Z66" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA66" t="s">
+      <c r="AA66" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB66" t="s">
         <v>104</v>
       </c>
-      <c r="AC66">
+      <c r="AD66">
         <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>94</v>
-      </c>
-      <c r="B67">
-        <v>259261.53</v>
-      </c>
-      <c r="C67">
-        <v>346507.55</v>
-      </c>
-      <c r="D67">
-        <v>310339.83</v>
-      </c>
-      <c r="E67">
-        <v>270786.08</v>
-      </c>
-      <c r="F67">
-        <v>224941.28</v>
-      </c>
-      <c r="G67">
-        <v>5</v>
-      </c>
-      <c r="H67" t="b">
-        <v>0</v>
-      </c>
-      <c r="I67">
-        <v>0.69069999999999998</v>
-      </c>
-      <c r="J67">
-        <v>267231.13267906482</v>
-      </c>
-      <c r="K67">
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="L67">
-        <v>0</v>
-      </c>
-      <c r="M67">
-        <v>4517.2220049124153</v>
-      </c>
-      <c r="N67" t="s">
-        <v>98</v>
-      </c>
-      <c r="O67">
-        <v>220420.74290606481</v>
-      </c>
-      <c r="P67">
-        <v>100134.7264341655</v>
-      </c>
-      <c r="Q67">
-        <v>220420.74290606481</v>
-      </c>
-      <c r="R67">
-        <v>296723.74749999988</v>
-      </c>
-      <c r="S67">
-        <v>282367.25400000002</v>
-      </c>
-      <c r="T67">
-        <v>-71782.467499999941</v>
-      </c>
-      <c r="U67">
-        <v>-0.2419168270311764</v>
-      </c>
-      <c r="V67">
-        <v>9.5674208367960131E-2</v>
-      </c>
-      <c r="X67" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y67" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z67" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA67" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC67">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>95</v>
-      </c>
-      <c r="B68">
-        <v>22.77</v>
-      </c>
-      <c r="C68">
-        <v>115787.2</v>
-      </c>
-      <c r="D68">
-        <v>65210.11</v>
-      </c>
-      <c r="E68">
-        <v>18382.03</v>
-      </c>
-      <c r="F68">
-        <v>-63098.82</v>
-      </c>
-      <c r="G68">
-        <v>5</v>
-      </c>
-      <c r="H68" t="b">
-        <v>0</v>
-      </c>
-      <c r="I68">
-        <v>0.99390000000000001</v>
-      </c>
-      <c r="J68">
-        <v>5477.9922713783963</v>
-      </c>
-      <c r="K68">
-        <v>0.998</v>
-      </c>
-      <c r="L68">
-        <v>0</v>
-      </c>
-      <c r="M68">
-        <v>-1215.905209574295</v>
-      </c>
-      <c r="N68" t="s">
-        <v>98</v>
-      </c>
-      <c r="O68">
-        <v>-61880.986149621611</v>
-      </c>
-      <c r="P68">
-        <v>-28111.853439353661</v>
-      </c>
-      <c r="Q68">
-        <v>-61880.986149621611</v>
-      </c>
-      <c r="R68">
-        <v>49850.527499999997</v>
-      </c>
-      <c r="S68">
-        <v>27260.657999999999</v>
-      </c>
-      <c r="T68">
-        <v>-112949.3475</v>
-      </c>
-      <c r="U68">
-        <v>-2.2657603272101778</v>
-      </c>
-      <c r="V68">
-        <v>0.89607171323153911</v>
-      </c>
-      <c r="X68" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y68" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z68" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA68" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC68">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: ensure 'Elasticity Classification' is extracted from Excel file during parsing
</commit_message>
<xml_diff>
--- a/public/expense-analysis.xlsx
+++ b/public/expense-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-gilliam-roanoke-1/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EA884EE-2DDB-B642-8476-9DFDE376C0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72AA1C73-BBA6-6142-AFFB-271A0347928A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="3440" windowWidth="25800" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -743,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
       <selection activeCell="Z41" sqref="Z41"/>
     </sheetView>
   </sheetViews>

</xml_diff>